<commit_message>
update more volunteers info
update more volunteers info
</commit_message>
<xml_diff>
--- a/campaign/VolunteerInformation.xlsx
+++ b/campaign/VolunteerInformation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="83">
   <si>
     <t>Name</t>
   </si>
@@ -247,6 +247,25 @@
   </si>
   <si>
     <t>Sufyan Azam</t>
+  </si>
+  <si>
+    <t>raghavs613@gmail.com</t>
+  </si>
+  <si>
+    <t>karticsharma74@hotmail.com</t>
+  </si>
+  <si>
+    <t>905 913 1216</t>
+  </si>
+  <si>
+    <t>ranbir_singh66@yahoo.ca</t>
+  </si>
+  <si>
+    <t>9057949737 / 
+6476220641</t>
+  </si>
+  <si>
+    <t>munvir_pannu@hotmail.com</t>
   </si>
 </sst>
 </file>
@@ -679,10 +698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1097,6 +1116,35 @@
       </c>
       <c r="E30">
         <v>9054860203</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="B31" t="s">
+        <v>77</v>
+      </c>
+      <c r="E31">
+        <v>9059131216</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="B32" t="s">
+        <v>78</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="B33" t="s">
+        <v>80</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5">
+      <c r="B34" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit volunteer information and sign list
commit volunteer information and sign list
</commit_message>
<xml_diff>
--- a/campaign/VolunteerInformation.xlsx
+++ b/campaign/VolunteerInformation.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="720" windowWidth="20780" windowHeight="14660"/>
+    <workbookView xWindow="720" yWindow="720" windowWidth="20775" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="92">
   <si>
     <t>SANIA HAIDER</t>
   </si>
@@ -295,13 +295,22 @@
   </si>
   <si>
     <t>647-774-3042</t>
+  </si>
+  <si>
+    <t>Sanah Khan</t>
+  </si>
+  <si>
+    <t>sanah.khan@mail.utoronto.ca</t>
+  </si>
+  <si>
+    <t>905-821-9984</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -370,6 +379,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -386,7 +463,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="7DE17D"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -662,22 +739,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:F35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -697,7 +774,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -717,7 +794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -734,7 +811,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -748,7 +825,7 @@
         <v>4165621762</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -763,7 +840,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -780,7 +857,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -797,7 +874,7 @@
         <v>6478600426</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -814,7 +891,7 @@
         <v>6477678445</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -831,7 +908,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -848,7 +925,7 @@
         <v>4166711521</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -865,7 +942,7 @@
         <v>6478295824</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -877,7 +954,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>72</v>
       </c>
@@ -894,7 +971,7 @@
         <v>9056731538</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>74</v>
       </c>
@@ -911,31 +988,31 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>53</v>
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>54</v>
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>55</v>
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>56</v>
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>80</v>
       </c>
@@ -946,19 +1023,19 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>58</v>
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>59</v>
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -975,7 +1052,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>66</v>
       </c>
@@ -987,7 +1064,7 @@
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>68</v>
       </c>
@@ -1004,7 +1081,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>78</v>
       </c>
@@ -1015,7 +1092,7 @@
         <v>9054619350</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -1032,7 +1109,7 @@
         <v>6474061810</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>82</v>
       </c>
@@ -1049,7 +1126,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>86</v>
       </c>
@@ -1063,7 +1140,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -1077,7 +1154,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -1091,7 +1168,7 @@
         <v>9054860203</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>10</v>
       </c>
@@ -1099,7 +1176,7 @@
         <v>9059131216</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>11</v>
       </c>
@@ -1107,7 +1184,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>15</v>
       </c>
@@ -1115,12 +1192,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -1132,6 +1209,20 @@
       </c>
       <c r="E35" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36" t="s">
+        <v>90</v>
+      </c>
+      <c r="D36" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1156,12 +1247,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1173,12 +1264,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
making changes and updates
making changes and updates
</commit_message>
<xml_diff>
--- a/campaign/VolunteerInformation.xlsx
+++ b/campaign/VolunteerInformation.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="100">
   <si>
     <t>SANIA HAIDER</t>
   </si>
@@ -319,6 +319,15 @@
   </si>
   <si>
     <t>289-633-2348</t>
+  </si>
+  <si>
+    <t>Michelle Bilek</t>
+  </si>
+  <si>
+    <t>NDP Erindale Candidate</t>
+  </si>
+  <si>
+    <t>mbilek@live.ca</t>
   </si>
 </sst>
 </file>
@@ -757,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,6 +1281,20 @@
         <v>289232516</v>
       </c>
     </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>97</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D39" t="s">
+        <v>98</v>
+      </c>
+      <c r="E39">
+        <v>4169535569</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -1283,6 +1306,7 @@
     <hyperlink ref="B7" r:id="rId6"/>
     <hyperlink ref="B30" r:id="rId7"/>
     <hyperlink ref="E6" r:id="rId8"/>
+    <hyperlink ref="B39" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Committing volunteer change and graphics
Committing volunteer change and graphics
</commit_message>
<xml_diff>
--- a/campaign/VolunteerInformation.xlsx
+++ b/campaign/VolunteerInformation.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-580" yWindow="-80" windowWidth="20740" windowHeight="11760"/>
+    <workbookView xWindow="-585" yWindow="-75" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -469,6 +469,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -485,7 +553,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="78DC78"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -763,19 +831,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1299,7 +1367,7 @@
         <v>4169535569</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="16">
+    <row r="40" spans="1:5" ht="17.25">
       <c r="A40" t="s">
         <v>20</v>
       </c>
@@ -1320,6 +1388,9 @@
       <c r="B41" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="E41">
+        <v>4167233866</v>
+      </c>
     </row>
     <row r="42" spans="1:5">
       <c r="B42" s="7" t="s">
@@ -1340,7 +1411,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="16">
+    <row r="44" spans="1:5" ht="17.25">
       <c r="A44" t="s">
         <v>27</v>
       </c>
@@ -1383,12 +1454,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1400,12 +1471,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Added new volunteer to list
</commit_message>
<xml_diff>
--- a/campaign/VolunteerInformation.xlsx
+++ b/campaign/VolunteerInformation.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-585" yWindow="-75" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="4760" yWindow="-80" windowWidth="21520" windowHeight="15400"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,129 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="118">
+  <si>
+    <t>ayesha.f13@gmail.com</t>
+  </si>
+  <si>
+    <t>Vivian Li</t>
+  </si>
+  <si>
+    <t>vivi881121@gmail.com</t>
+  </si>
+  <si>
+    <t>Diya</t>
+  </si>
+  <si>
+    <t>diyakamath@yahoo.ca</t>
+  </si>
+  <si>
+    <t>Stephen Lewis Secondary</t>
+  </si>
+  <si>
+    <t>David Suzuki Secondary</t>
+  </si>
+  <si>
+    <t>Contact Number</t>
+  </si>
+  <si>
+    <t>annie.195@hotmail.com</t>
+  </si>
+  <si>
+    <t>fatehhayer1999@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> hawkstar@live.ca</t>
+  </si>
+  <si>
+    <t>mikayla_december@outlook.com</t>
+  </si>
+  <si>
+    <t>imranshaista@hotmail.com</t>
+  </si>
+  <si>
+    <t>sundaram_balas@yahoo.ca</t>
+  </si>
+  <si>
+    <t>taimoorgul98@gmail.com</t>
+  </si>
+  <si>
+    <t>mmdj360@gmail.com</t>
+  </si>
+  <si>
+    <t>Xenwraith@gmail.com</t>
+  </si>
+  <si>
+    <t>Jordan Gray</t>
+  </si>
+  <si>
+    <t>jordancgray@hotmail.com</t>
+  </si>
+  <si>
+    <t>(647) 233-4244</t>
+  </si>
+  <si>
+    <t>416-737-7706 / 647-767-9601</t>
+  </si>
+  <si>
+    <t>416-738-3281</t>
+  </si>
+  <si>
+    <t>Drive</t>
+  </si>
+  <si>
+    <t>Syed Abdullah Hussain</t>
+  </si>
+  <si>
+    <t>abd_pisces@live.com</t>
+  </si>
+  <si>
+    <t>Dylan Leonard</t>
+  </si>
+  <si>
+    <t>647 783 6844</t>
+  </si>
+  <si>
+    <t>dy2_leonard@hotmail.com</t>
+  </si>
+  <si>
+    <t>Anisha Akhtar</t>
+  </si>
+  <si>
+    <t>York University</t>
+  </si>
+  <si>
+    <t>Fateh Hayer</t>
+  </si>
+  <si>
+    <t>David Suzuki Secondary School, Brampton</t>
+  </si>
+  <si>
+    <t>jetaix01@yahoo.ca</t>
+  </si>
+  <si>
+    <t>fawaddv@gmail.com</t>
+  </si>
+  <si>
+    <t>Taimoor</t>
+  </si>
+  <si>
+    <t>647-300-0101 / 647 960 1002</t>
+  </si>
+  <si>
+    <t>tanvi1111@hotmail.com</t>
+  </si>
+  <si>
+    <t>Tanvi Mehta</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gordon Graydon Memorial Secondary School</t>
+  </si>
+  <si>
+    <t>(647) 502-3605</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
   <si>
     <t>905-956-2182</t>
   </si>
@@ -271,121 +393,13 @@
   </si>
   <si>
     <t>Ayesha Faizi</t>
-  </si>
-  <si>
-    <t>ayesha.f13@gmail.com</t>
-  </si>
-  <si>
-    <t>Vivian Li</t>
-  </si>
-  <si>
-    <t>vivi881121@gmail.com</t>
-  </si>
-  <si>
-    <t>Diya</t>
-  </si>
-  <si>
-    <t>diyakamath@yahoo.ca</t>
-  </si>
-  <si>
-    <t>Stephen Lewis Secondary</t>
-  </si>
-  <si>
-    <t>David Suzuki Secondary</t>
-  </si>
-  <si>
-    <t>Contact Number</t>
-  </si>
-  <si>
-    <t>annie.195@hotmail.com</t>
-  </si>
-  <si>
-    <t>fatehhayer1999@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> hawkstar@live.ca</t>
-  </si>
-  <si>
-    <t>mikayla_december@outlook.com</t>
-  </si>
-  <si>
-    <t>imranshaista@hotmail.com</t>
-  </si>
-  <si>
-    <t>sundaram_balas@yahoo.ca</t>
-  </si>
-  <si>
-    <t>taimoorgul98@gmail.com</t>
-  </si>
-  <si>
-    <t>mmdj360@gmail.com</t>
-  </si>
-  <si>
-    <t>Xenwraith@gmail.com</t>
-  </si>
-  <si>
-    <t>Jordan Gray</t>
-  </si>
-  <si>
-    <t>jordancgray@hotmail.com</t>
-  </si>
-  <si>
-    <t>(647) 233-4244</t>
-  </si>
-  <si>
-    <t>416-737-7706 / 647-767-9601</t>
-  </si>
-  <si>
-    <t>416-738-3281</t>
-  </si>
-  <si>
-    <t>Drive</t>
-  </si>
-  <si>
-    <t>Syed Abdullah Hussain</t>
-  </si>
-  <si>
-    <t>abd_pisces@live.com</t>
-  </si>
-  <si>
-    <t>Dylan Leonard</t>
-  </si>
-  <si>
-    <t>647 783 6844</t>
-  </si>
-  <si>
-    <t>dy2_leonard@hotmail.com</t>
-  </si>
-  <si>
-    <t>Anisha Akhtar</t>
-  </si>
-  <si>
-    <t>York University</t>
-  </si>
-  <si>
-    <t>Fateh Hayer</t>
-  </si>
-  <si>
-    <t>David Suzuki Secondary School, Brampton</t>
-  </si>
-  <si>
-    <t>jetaix01@yahoo.ca</t>
-  </si>
-  <si>
-    <t>fawaddv@gmail.com</t>
-  </si>
-  <si>
-    <t>Taimoor</t>
-  </si>
-  <si>
-    <t>647-300-0101 / 647 960 1002</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -425,6 +439,16 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="21"/>
+      <name val="Tahoma"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="63"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -447,7 +471,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -462,6 +486,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -469,74 +495,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -553,7 +511,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="7DE17D"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -831,53 +789,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="D1" t="s">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="E1" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
       <c r="C2">
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="E2" s="2">
         <v>6472445427</v>
@@ -886,29 +844,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="C3">
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>104</v>
       </c>
       <c r="C4">
         <v>17</v>
@@ -917,515 +875,532 @@
         <v>4165621762</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>105</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>106</v>
       </c>
       <c r="C5">
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>83</v>
+        <v>5</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>107</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>68</v>
+        <v>108</v>
       </c>
       <c r="C6">
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>69</v>
+        <v>109</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>71</v>
+        <v>111</v>
       </c>
       <c r="C7">
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>84</v>
+        <v>6</v>
       </c>
       <c r="E7" s="2">
         <v>6478600426</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>112</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>113</v>
       </c>
       <c r="C8">
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>74</v>
+        <v>114</v>
       </c>
       <c r="E8" s="2">
         <v>6477678445</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>115</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>116</v>
       </c>
       <c r="C9">
         <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>77</v>
+        <v>117</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="C10">
         <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="E10" s="2">
         <v>4166711521</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>2</v>
       </c>
       <c r="C11">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>74</v>
+        <v>114</v>
       </c>
       <c r="E11" s="2">
         <v>6478295824</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>81</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>82</v>
+        <v>4</v>
       </c>
       <c r="C12">
         <v>14</v>
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>106</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>86</v>
+        <v>8</v>
       </c>
       <c r="C13">
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>107</v>
+        <v>29</v>
       </c>
       <c r="E13" s="2">
         <v>9056731538</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>108</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>87</v>
+        <v>9</v>
       </c>
       <c r="C14">
         <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>109</v>
+        <v>31</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="B15" t="s">
-        <v>88</v>
+        <v>10</v>
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="B16" t="s">
-        <v>89</v>
+        <v>11</v>
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="B17" s="1" t="s">
-        <v>90</v>
+        <v>12</v>
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="B18" t="s">
-        <v>91</v>
+        <v>13</v>
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>112</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>92</v>
+        <v>14</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="B20" s="1" t="s">
-        <v>93</v>
+        <v>15</v>
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="B21" t="s">
-        <v>94</v>
+        <v>16</v>
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>95</v>
+        <v>17</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>96</v>
+        <v>18</v>
       </c>
       <c r="C22">
         <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>101</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>102</v>
+        <v>24</v>
       </c>
       <c r="C23">
         <v>14</v>
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>103</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>105</v>
+        <v>27</v>
       </c>
       <c r="C24">
         <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>110</v>
+        <v>32</v>
       </c>
       <c r="C25">
         <v>13</v>
       </c>
       <c r="D25" t="s">
-        <v>34</v>
+        <v>74</v>
       </c>
       <c r="E25">
         <v>9054619350</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="B26" t="s">
-        <v>111</v>
+        <v>33</v>
       </c>
       <c r="C26">
         <v>13</v>
       </c>
       <c r="D26" t="s">
-        <v>48</v>
+        <v>88</v>
       </c>
       <c r="E26">
         <v>6474061810</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="5" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="C27">
         <v>17</v>
       </c>
       <c r="D27" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="5" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="B28" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D28" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="B29" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="D29" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="D30" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="E30">
         <v>9054860203</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="B31" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="E31">
         <v>9059131216</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="B32" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="E32" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="B33" t="s">
+        <v>90</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="B34" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" t="s">
+        <v>81</v>
+      </c>
+      <c r="D35" t="s">
+        <v>82</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+      <c r="D36" t="s">
+        <v>101</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E33" s="2" t="s">
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>40</v>
-      </c>
-      <c r="B35" t="s">
-        <v>41</v>
-      </c>
-      <c r="D35" t="s">
-        <v>42</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>8</v>
-      </c>
-      <c r="B36" t="s">
-        <v>9</v>
-      </c>
-      <c r="D36" t="s">
-        <v>61</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>13</v>
-      </c>
-      <c r="B37" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" t="s">
-        <v>12</v>
       </c>
       <c r="E37">
         <v>9058907919</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="B38" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="D38" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="E38">
         <v>289232516</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="D39" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="E39">
         <v>4169535569</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="16">
       <c r="A40" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="C40">
         <v>21</v>
       </c>
       <c r="D40" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="E40" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="B41" s="7" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="E41">
         <v>4167233866</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="B42" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="C43">
         <v>15</v>
       </c>
       <c r="D43" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="16">
       <c r="A44" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="C44">
         <v>21</v>
       </c>
       <c r="D44" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="E44" t="s">
-        <v>31</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>37</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45">
+        <v>14</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1454,12 +1429,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1471,12 +1446,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Added data entry volunteers to list
</commit_message>
<xml_diff>
--- a/campaign/VolunteerInformation.xlsx
+++ b/campaign/VolunteerInformation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4760" yWindow="-80" windowWidth="21520" windowHeight="15400"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="21520" windowHeight="15400"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,252 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="118">
-  <si>
-    <t>ayesha.f13@gmail.com</t>
-  </si>
-  <si>
-    <t>Vivian Li</t>
-  </si>
-  <si>
-    <t>vivi881121@gmail.com</t>
-  </si>
-  <si>
-    <t>Diya</t>
-  </si>
-  <si>
-    <t>diyakamath@yahoo.ca</t>
-  </si>
-  <si>
-    <t>Stephen Lewis Secondary</t>
-  </si>
-  <si>
-    <t>David Suzuki Secondary</t>
-  </si>
-  <si>
-    <t>Contact Number</t>
-  </si>
-  <si>
-    <t>annie.195@hotmail.com</t>
-  </si>
-  <si>
-    <t>fatehhayer1999@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> hawkstar@live.ca</t>
-  </si>
-  <si>
-    <t>mikayla_december@outlook.com</t>
-  </si>
-  <si>
-    <t>imranshaista@hotmail.com</t>
-  </si>
-  <si>
-    <t>sundaram_balas@yahoo.ca</t>
-  </si>
-  <si>
-    <t>taimoorgul98@gmail.com</t>
-  </si>
-  <si>
-    <t>mmdj360@gmail.com</t>
-  </si>
-  <si>
-    <t>Xenwraith@gmail.com</t>
-  </si>
-  <si>
-    <t>Jordan Gray</t>
-  </si>
-  <si>
-    <t>jordancgray@hotmail.com</t>
-  </si>
-  <si>
-    <t>(647) 233-4244</t>
-  </si>
-  <si>
-    <t>416-737-7706 / 647-767-9601</t>
-  </si>
-  <si>
-    <t>416-738-3281</t>
-  </si>
-  <si>
-    <t>Drive</t>
-  </si>
-  <si>
-    <t>Syed Abdullah Hussain</t>
-  </si>
-  <si>
-    <t>abd_pisces@live.com</t>
-  </si>
-  <si>
-    <t>Dylan Leonard</t>
-  </si>
-  <si>
-    <t>647 783 6844</t>
-  </si>
-  <si>
-    <t>dy2_leonard@hotmail.com</t>
-  </si>
-  <si>
-    <t>Anisha Akhtar</t>
-  </si>
-  <si>
-    <t>York University</t>
-  </si>
-  <si>
-    <t>Fateh Hayer</t>
-  </si>
-  <si>
-    <t>David Suzuki Secondary School, Brampton</t>
-  </si>
-  <si>
-    <t>jetaix01@yahoo.ca</t>
-  </si>
-  <si>
-    <t>fawaddv@gmail.com</t>
-  </si>
-  <si>
-    <t>Taimoor</t>
-  </si>
-  <si>
-    <t>647-300-0101 / 647 960 1002</t>
-  </si>
-  <si>
-    <t>tanvi1111@hotmail.com</t>
-  </si>
-  <si>
-    <t>Tanvi Mehta</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gordon Graydon Memorial Secondary School</t>
-  </si>
-  <si>
-    <t>(647) 502-3605</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>905-956-2182</t>
-  </si>
-  <si>
-    <t>Drishti Thakkar</t>
-  </si>
-  <si>
-    <t>drishti.thakkar@gmail.com</t>
-  </si>
-  <si>
-    <t>Port Credit Secondary</t>
-  </si>
-  <si>
-    <t>647-390-9063</t>
-  </si>
-  <si>
-    <t>Ujala Feroze</t>
-  </si>
-  <si>
-    <t>ujala.feroze@mail.utoronto.ca</t>
-  </si>
-  <si>
-    <t>647-774-3042</t>
-  </si>
-  <si>
-    <t>Sanah Khan</t>
-  </si>
-  <si>
-    <t>sanah.khan@mail.utoronto.ca</t>
-  </si>
-  <si>
-    <t>905-821-9984</t>
-  </si>
-  <si>
-    <t>inleonard22@gmail.com</t>
-  </si>
-  <si>
-    <t>MMYL</t>
-  </si>
-  <si>
-    <t>Alan Leonard</t>
-  </si>
-  <si>
-    <t>jz1998119@hotmail.com</t>
-  </si>
-  <si>
-    <t>Jason Z</t>
-  </si>
-  <si>
-    <t>289-633-2348</t>
-  </si>
-  <si>
-    <t>Michelle Bilek</t>
-  </si>
-  <si>
-    <t>NDP Erindale Candidate</t>
-  </si>
-  <si>
-    <t>mbilek@live.ca</t>
-  </si>
-  <si>
-    <t>Ke Zhang (Coco)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ke.coco.zhang@gmail.com</t>
-  </si>
-  <si>
-    <t>Humber Lakeshore</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>(647) 888-8744</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>hamzakhan17@hotmail.com</t>
-  </si>
-  <si>
-    <t>unb1975@yahoo.ca</t>
-  </si>
-  <si>
-    <t>wajeehkhan123@hotmail.com</t>
-  </si>
-  <si>
-    <t>Amreet Singh</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>amreet93sidhu@gmail.com</t>
-  </si>
-  <si>
-    <t>Wajeeh Amir Khan</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rick Hansen Secondary School</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>(647) 822-7275</t>
-  </si>
-  <si>
-    <t>Sheridan</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Zayd Siddiqui</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>David Leeder Middle School</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SANIA HAIDER</t>
-  </si>
-  <si>
-    <t>sania.haider@mail.utoronto.ca</t>
-  </si>
-  <si>
-    <t>(647) 282-8452</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="125">
   <si>
     <t>afi_capk@hotmail.com</t>
   </si>
@@ -393,13 +148,281 @@
   </si>
   <si>
     <t>Ayesha Faizi</t>
+  </si>
+  <si>
+    <t>Ali Turab Lotia</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>aliturablotia@gmail.com</t>
+  </si>
+  <si>
+    <t>647-997-085</t>
+  </si>
+  <si>
+    <t>Paul Konieczny</t>
+  </si>
+  <si>
+    <t>647-217-2793</t>
+  </si>
+  <si>
+    <t>pkonieczny@rogers.com</t>
+  </si>
+  <si>
+    <t>UTM</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ayesha.f13@gmail.com</t>
+  </si>
+  <si>
+    <t>Vivian Li</t>
+  </si>
+  <si>
+    <t>vivi881121@gmail.com</t>
+  </si>
+  <si>
+    <t>Diya</t>
+  </si>
+  <si>
+    <t>diyakamath@yahoo.ca</t>
+  </si>
+  <si>
+    <t>Stephen Lewis Secondary</t>
+  </si>
+  <si>
+    <t>David Suzuki Secondary</t>
+  </si>
+  <si>
+    <t>Contact Number</t>
+  </si>
+  <si>
+    <t>annie.195@hotmail.com</t>
+  </si>
+  <si>
+    <t>fatehhayer1999@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> hawkstar@live.ca</t>
+  </si>
+  <si>
+    <t>mikayla_december@outlook.com</t>
+  </si>
+  <si>
+    <t>imranshaista@hotmail.com</t>
+  </si>
+  <si>
+    <t>sundaram_balas@yahoo.ca</t>
+  </si>
+  <si>
+    <t>taimoorgul98@gmail.com</t>
+  </si>
+  <si>
+    <t>mmdj360@gmail.com</t>
+  </si>
+  <si>
+    <t>Xenwraith@gmail.com</t>
+  </si>
+  <si>
+    <t>Jordan Gray</t>
+  </si>
+  <si>
+    <t>jordancgray@hotmail.com</t>
+  </si>
+  <si>
+    <t>(647) 233-4244</t>
+  </si>
+  <si>
+    <t>416-737-7706 / 647-767-9601</t>
+  </si>
+  <si>
+    <t>416-738-3281</t>
+  </si>
+  <si>
+    <t>Drive</t>
+  </si>
+  <si>
+    <t>Syed Abdullah Hussain</t>
+  </si>
+  <si>
+    <t>abd_pisces@live.com</t>
+  </si>
+  <si>
+    <t>Dylan Leonard</t>
+  </si>
+  <si>
+    <t>647 783 6844</t>
+  </si>
+  <si>
+    <t>dy2_leonard@hotmail.com</t>
+  </si>
+  <si>
+    <t>Anisha Akhtar</t>
+  </si>
+  <si>
+    <t>York University</t>
+  </si>
+  <si>
+    <t>Fateh Hayer</t>
+  </si>
+  <si>
+    <t>David Suzuki Secondary School, Brampton</t>
+  </si>
+  <si>
+    <t>jetaix01@yahoo.ca</t>
+  </si>
+  <si>
+    <t>fawaddv@gmail.com</t>
+  </si>
+  <si>
+    <t>Taimoor</t>
+  </si>
+  <si>
+    <t>647-300-0101 / 647 960 1002</t>
+  </si>
+  <si>
+    <t>tanvi1111@hotmail.com</t>
+  </si>
+  <si>
+    <t>Tanvi Mehta</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gordon Graydon Memorial Secondary School</t>
+  </si>
+  <si>
+    <t>(647) 502-3605</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>905-956-2182</t>
+  </si>
+  <si>
+    <t>Drishti Thakkar</t>
+  </si>
+  <si>
+    <t>drishti.thakkar@gmail.com</t>
+  </si>
+  <si>
+    <t>Port Credit Secondary</t>
+  </si>
+  <si>
+    <t>647-390-9063</t>
+  </si>
+  <si>
+    <t>Ujala Feroze</t>
+  </si>
+  <si>
+    <t>ujala.feroze@mail.utoronto.ca</t>
+  </si>
+  <si>
+    <t>647-774-3042</t>
+  </si>
+  <si>
+    <t>Sanah Khan</t>
+  </si>
+  <si>
+    <t>sanah.khan@mail.utoronto.ca</t>
+  </si>
+  <si>
+    <t>905-821-9984</t>
+  </si>
+  <si>
+    <t>inleonard22@gmail.com</t>
+  </si>
+  <si>
+    <t>MMYL</t>
+  </si>
+  <si>
+    <t>Alan Leonard</t>
+  </si>
+  <si>
+    <t>jz1998119@hotmail.com</t>
+  </si>
+  <si>
+    <t>Jason Z</t>
+  </si>
+  <si>
+    <t>289-633-2348</t>
+  </si>
+  <si>
+    <t>Michelle Bilek</t>
+  </si>
+  <si>
+    <t>NDP Erindale Candidate</t>
+  </si>
+  <si>
+    <t>mbilek@live.ca</t>
+  </si>
+  <si>
+    <t>Ke Zhang (Coco)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ke.coco.zhang@gmail.com</t>
+  </si>
+  <si>
+    <t>Humber Lakeshore</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(647) 888-8744</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>hamzakhan17@hotmail.com</t>
+  </si>
+  <si>
+    <t>unb1975@yahoo.ca</t>
+  </si>
+  <si>
+    <t>wajeehkhan123@hotmail.com</t>
+  </si>
+  <si>
+    <t>Amreet Singh</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>amreet93sidhu@gmail.com</t>
+  </si>
+  <si>
+    <t>Wajeeh Amir Khan</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rick Hansen Secondary School</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(647) 822-7275</t>
+  </si>
+  <si>
+    <t>Sheridan</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zayd Siddiqui</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>David Leeder Middle School</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SANIA HAIDER</t>
+  </si>
+  <si>
+    <t>sania.haider@mail.utoronto.ca</t>
+  </si>
+  <si>
+    <t>(647) 282-8452</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -449,6 +472,16 @@
       <color indexed="63"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="15"/>
+      <color indexed="63"/>
+      <name val="Tahoma"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color indexed="18"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -471,7 +504,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -488,6 +521,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -790,10 +825,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -806,36 +841,36 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>95</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>96</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>101</v>
+        <v>23</v>
       </c>
       <c r="E2" s="2">
         <v>6472445427</v>
@@ -846,27 +881,27 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>102</v>
+        <v>24</v>
       </c>
       <c r="C3">
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>101</v>
+        <v>23</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>104</v>
+        <v>26</v>
       </c>
       <c r="C4">
         <v>17</v>
@@ -877,50 +912,50 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>28</v>
       </c>
       <c r="C5">
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>56</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>107</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>108</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>109</v>
+        <v>31</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>111</v>
+        <v>33</v>
       </c>
       <c r="C7">
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="E7" s="2">
         <v>6478600426</v>
@@ -928,16 +963,16 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>112</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="C8">
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>114</v>
+        <v>36</v>
       </c>
       <c r="E8" s="2">
         <v>6477678445</v>
@@ -945,33 +980,33 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>116</v>
+        <v>38</v>
       </c>
       <c r="C9">
         <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>101</v>
+        <v>23</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>91</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>117</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="C10">
         <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>101</v>
+        <v>23</v>
       </c>
       <c r="E10" s="2">
         <v>4166711521</v>
@@ -979,16 +1014,16 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="C11">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>114</v>
+        <v>36</v>
       </c>
       <c r="E11" s="2">
         <v>6478295824</v>
@@ -996,10 +1031,10 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="C12">
         <v>14</v>
@@ -1008,16 +1043,16 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="C13">
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="E13" s="2">
         <v>9056731538</v>
@@ -1025,91 +1060,91 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="C14">
         <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="B15" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:6">
       <c r="B16" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5">
       <c r="B17" s="1" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5">
       <c r="B18" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>40</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="B20" s="1" t="s">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5">
       <c r="B21" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="C22">
         <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="C23">
         <v>14</v>
@@ -1118,33 +1153,33 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="C24">
         <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="C25">
         <v>13</v>
       </c>
       <c r="D25" t="s">
-        <v>74</v>
+        <v>121</v>
       </c>
       <c r="E25">
         <v>9054619350</v>
@@ -1152,16 +1187,16 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="C26">
         <v>13</v>
       </c>
       <c r="D26" t="s">
-        <v>88</v>
+        <v>10</v>
       </c>
       <c r="E26">
         <v>6474061810</v>
@@ -1169,58 +1204,58 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="5" t="s">
-        <v>41</v>
+        <v>88</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="C27">
         <v>17</v>
       </c>
       <c r="D27" t="s">
-        <v>43</v>
+        <v>90</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>44</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="5" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="B28" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="D28" t="s">
-        <v>101</v>
+        <v>23</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>47</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>75</v>
+        <v>122</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
+        <v>123</v>
       </c>
       <c r="D29" t="s">
-        <v>101</v>
+        <v>23</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>77</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>6</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="D30" t="s">
-        <v>79</v>
+        <v>1</v>
       </c>
       <c r="E30">
         <v>9054860203</v>
@@ -1228,7 +1263,7 @@
     </row>
     <row r="31" spans="1:5">
       <c r="B31" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="E31">
         <v>9059131216</v>
@@ -1236,62 +1271,62 @@
     </row>
     <row r="32" spans="1:5">
       <c r="B32" t="s">
-        <v>86</v>
+        <v>8</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>89</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="B33" t="s">
-        <v>90</v>
+        <v>12</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>92</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="B34" t="s">
-        <v>93</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>80</v>
+        <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>81</v>
+        <v>3</v>
       </c>
       <c r="D35" t="s">
-        <v>82</v>
+        <v>4</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>83</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>95</v>
       </c>
       <c r="B36" t="s">
-        <v>49</v>
+        <v>96</v>
       </c>
       <c r="D36" t="s">
-        <v>101</v>
+        <v>23</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>50</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>100</v>
       </c>
       <c r="B37" t="s">
-        <v>51</v>
+        <v>98</v>
       </c>
       <c r="D37" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="E37">
         <v>9058907919</v>
@@ -1299,13 +1334,13 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>55</v>
+        <v>102</v>
       </c>
       <c r="B38" t="s">
-        <v>54</v>
+        <v>101</v>
       </c>
       <c r="D38" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="E38">
         <v>289232516</v>
@@ -1313,13 +1348,13 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>57</v>
+        <v>104</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>59</v>
+        <v>106</v>
       </c>
       <c r="D39" t="s">
-        <v>58</v>
+        <v>105</v>
       </c>
       <c r="E39">
         <v>4169535569</v>
@@ -1327,24 +1362,24 @@
     </row>
     <row r="40" spans="1:5" ht="16">
       <c r="A40" t="s">
-        <v>60</v>
+        <v>107</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
       <c r="C40">
         <v>21</v>
       </c>
       <c r="D40" t="s">
-        <v>62</v>
+        <v>109</v>
       </c>
       <c r="E40" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="B41" s="7" t="s">
-        <v>64</v>
+        <v>111</v>
       </c>
       <c r="E41">
         <v>4167233866</v>
@@ -1352,55 +1387,83 @@
     </row>
     <row r="42" spans="1:5">
       <c r="B42" s="7" t="s">
-        <v>65</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>69</v>
+        <v>116</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>66</v>
+        <v>113</v>
       </c>
       <c r="C43">
         <v>15</v>
       </c>
       <c r="D43" t="s">
-        <v>70</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="16">
       <c r="A44" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>68</v>
+        <v>115</v>
       </c>
       <c r="C44">
         <v>21</v>
       </c>
       <c r="D44" t="s">
-        <v>72</v>
+        <v>119</v>
       </c>
       <c r="E44" t="s">
-        <v>71</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>37</v>
+        <v>84</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>36</v>
+        <v>83</v>
       </c>
       <c r="C45">
         <v>14</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>38</v>
+        <v>85</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>39</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="19">
+      <c r="A46" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D46" t="s">
+        <v>46</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="16">
+      <c r="A47" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D47" t="s">
+        <v>46</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1418,6 +1481,8 @@
     <hyperlink ref="B41" r:id="rId10"/>
     <hyperlink ref="B42" r:id="rId11"/>
     <hyperlink ref="B43" r:id="rId12"/>
+    <hyperlink ref="B46" r:id="rId13"/>
+    <hyperlink ref="B47" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Added Ammar to volunteer list
</commit_message>
<xml_diff>
--- a/campaign/VolunteerInformation.xlsx
+++ b/campaign/VolunteerInformation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="21520" windowHeight="15400"/>
+    <workbookView xWindow="2140" yWindow="2460" windowWidth="21520" windowHeight="15400"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,166 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="128">
+  <si>
+    <t>jetaix01@yahoo.ca</t>
+  </si>
+  <si>
+    <t>fawaddv@gmail.com</t>
+  </si>
+  <si>
+    <t>Taimoor</t>
+  </si>
+  <si>
+    <t>647-300-0101 / 647 960 1002</t>
+  </si>
+  <si>
+    <t>tanvi1111@hotmail.com</t>
+  </si>
+  <si>
+    <t>Tanvi Mehta</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gordon Graydon Memorial Secondary School</t>
+  </si>
+  <si>
+    <t>(647) 502-3605</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>905-956-2182</t>
+  </si>
+  <si>
+    <t>Drishti Thakkar</t>
+  </si>
+  <si>
+    <t>drishti.thakkar@gmail.com</t>
+  </si>
+  <si>
+    <t>Port Credit Secondary</t>
+  </si>
+  <si>
+    <t>647-390-9063</t>
+  </si>
+  <si>
+    <t>Ujala Feroze</t>
+  </si>
+  <si>
+    <t>ujala.feroze@mail.utoronto.ca</t>
+  </si>
+  <si>
+    <t>647-774-3042</t>
+  </si>
+  <si>
+    <t>Sanah Khan</t>
+  </si>
+  <si>
+    <t>sanah.khan@mail.utoronto.ca</t>
+  </si>
+  <si>
+    <t>905-821-9984</t>
+  </si>
+  <si>
+    <t>inleonard22@gmail.com</t>
+  </si>
+  <si>
+    <t>MMYL</t>
+  </si>
+  <si>
+    <t>Alan Leonard</t>
+  </si>
+  <si>
+    <t>jz1998119@hotmail.com</t>
+  </si>
+  <si>
+    <t>Jason Z</t>
+  </si>
+  <si>
+    <t>289-633-2348</t>
+  </si>
+  <si>
+    <t>Michelle Bilek</t>
+  </si>
+  <si>
+    <t>NDP Erindale Candidate</t>
+  </si>
+  <si>
+    <t>mbilek@live.ca</t>
+  </si>
+  <si>
+    <t>Ke Zhang (Coco)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ke.coco.zhang@gmail.com</t>
+  </si>
+  <si>
+    <t>Humber Lakeshore</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(647) 888-8744</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>hamzakhan17@hotmail.com</t>
+  </si>
+  <si>
+    <t>unb1975@yahoo.ca</t>
+  </si>
+  <si>
+    <t>wajeehkhan123@hotmail.com</t>
+  </si>
+  <si>
+    <t>Amreet Singh</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>amreet93sidhu@gmail.com</t>
+  </si>
+  <si>
+    <t>Wajeeh Amir Khan</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rick Hansen Secondary School</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(647) 822-7275</t>
+  </si>
+  <si>
+    <t>Sheridan</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zayd Siddiqui</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>David Leeder Middle School</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SANIA HAIDER</t>
+  </si>
+  <si>
+    <t>sania.haider@mail.utoronto.ca</t>
+  </si>
+  <si>
+    <t>(647) 282-8452</t>
+  </si>
+  <si>
+    <t>arrafaqat@gmail.com</t>
+  </si>
+  <si>
+    <t>Ammar Rafaqat</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Acension Of Our Lord S.S.</t>
+  </si>
   <si>
     <t>afi_capk@hotmail.com</t>
   </si>
@@ -267,162 +426,13 @@
   </si>
   <si>
     <t>David Suzuki Secondary School, Brampton</t>
-  </si>
-  <si>
-    <t>jetaix01@yahoo.ca</t>
-  </si>
-  <si>
-    <t>fawaddv@gmail.com</t>
-  </si>
-  <si>
-    <t>Taimoor</t>
-  </si>
-  <si>
-    <t>647-300-0101 / 647 960 1002</t>
-  </si>
-  <si>
-    <t>tanvi1111@hotmail.com</t>
-  </si>
-  <si>
-    <t>Tanvi Mehta</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gordon Graydon Memorial Secondary School</t>
-  </si>
-  <si>
-    <t>(647) 502-3605</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>905-956-2182</t>
-  </si>
-  <si>
-    <t>Drishti Thakkar</t>
-  </si>
-  <si>
-    <t>drishti.thakkar@gmail.com</t>
-  </si>
-  <si>
-    <t>Port Credit Secondary</t>
-  </si>
-  <si>
-    <t>647-390-9063</t>
-  </si>
-  <si>
-    <t>Ujala Feroze</t>
-  </si>
-  <si>
-    <t>ujala.feroze@mail.utoronto.ca</t>
-  </si>
-  <si>
-    <t>647-774-3042</t>
-  </si>
-  <si>
-    <t>Sanah Khan</t>
-  </si>
-  <si>
-    <t>sanah.khan@mail.utoronto.ca</t>
-  </si>
-  <si>
-    <t>905-821-9984</t>
-  </si>
-  <si>
-    <t>inleonard22@gmail.com</t>
-  </si>
-  <si>
-    <t>MMYL</t>
-  </si>
-  <si>
-    <t>Alan Leonard</t>
-  </si>
-  <si>
-    <t>jz1998119@hotmail.com</t>
-  </si>
-  <si>
-    <t>Jason Z</t>
-  </si>
-  <si>
-    <t>289-633-2348</t>
-  </si>
-  <si>
-    <t>Michelle Bilek</t>
-  </si>
-  <si>
-    <t>NDP Erindale Candidate</t>
-  </si>
-  <si>
-    <t>mbilek@live.ca</t>
-  </si>
-  <si>
-    <t>Ke Zhang (Coco)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ke.coco.zhang@gmail.com</t>
-  </si>
-  <si>
-    <t>Humber Lakeshore</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>(647) 888-8744</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>hamzakhan17@hotmail.com</t>
-  </si>
-  <si>
-    <t>unb1975@yahoo.ca</t>
-  </si>
-  <si>
-    <t>wajeehkhan123@hotmail.com</t>
-  </si>
-  <si>
-    <t>Amreet Singh</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>amreet93sidhu@gmail.com</t>
-  </si>
-  <si>
-    <t>Wajeeh Amir Khan</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rick Hansen Secondary School</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>(647) 822-7275</t>
-  </si>
-  <si>
-    <t>Sheridan</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Zayd Siddiqui</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>David Leeder Middle School</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SANIA HAIDER</t>
-  </si>
-  <si>
-    <t>sania.haider@mail.utoronto.ca</t>
-  </si>
-  <si>
-    <t>(647) 282-8452</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -482,6 +492,11 @@
       <color indexed="18"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="21"/>
+      <name val="Tahoma"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -504,7 +519,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -523,6 +538,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -825,7 +841,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D48" sqref="D48"/>
@@ -841,36 +857,36 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="E1" t="s">
-        <v>54</v>
+        <v>103</v>
       </c>
       <c r="F1" t="s">
-        <v>69</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="C2">
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="E2" s="2">
         <v>6472445427</v>
@@ -881,27 +897,27 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="C3">
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>68</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="C4">
         <v>17</v>
@@ -912,50 +928,50 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="C5">
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>101</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>103</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>79</v>
       </c>
       <c r="C6">
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>67</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>82</v>
       </c>
       <c r="C7">
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="E7" s="2">
         <v>6478600426</v>
@@ -963,16 +979,16 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>83</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>84</v>
       </c>
       <c r="C8">
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="E8" s="2">
         <v>6477678445</v>
@@ -980,33 +996,33 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>87</v>
       </c>
       <c r="C9">
         <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>88</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>96</v>
       </c>
       <c r="C10">
         <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="E10" s="2">
         <v>4166711521</v>
@@ -1014,16 +1030,16 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>98</v>
       </c>
       <c r="C11">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="E11" s="2">
         <v>6478295824</v>
@@ -1031,10 +1047,10 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="C12">
         <v>14</v>
@@ -1043,16 +1059,16 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>124</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>55</v>
+        <v>104</v>
       </c>
       <c r="C13">
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>76</v>
+        <v>125</v>
       </c>
       <c r="E13" s="2">
         <v>9056731538</v>
@@ -1060,91 +1076,91 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>126</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>105</v>
       </c>
       <c r="C14">
         <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>78</v>
+        <v>127</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="B15" t="s">
-        <v>57</v>
+        <v>106</v>
       </c>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:6">
       <c r="B16" t="s">
-        <v>58</v>
+        <v>107</v>
       </c>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5">
       <c r="B17" s="1" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5">
       <c r="B18" t="s">
-        <v>60</v>
+        <v>109</v>
       </c>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>81</v>
+        <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>110</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>87</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="B20" s="1" t="s">
-        <v>62</v>
+        <v>111</v>
       </c>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5">
       <c r="B21" t="s">
-        <v>63</v>
+        <v>112</v>
       </c>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>113</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>65</v>
+        <v>114</v>
       </c>
       <c r="C22">
         <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>99</v>
+        <v>20</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>66</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>119</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>120</v>
       </c>
       <c r="C23">
         <v>14</v>
@@ -1153,33 +1169,33 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>72</v>
+        <v>121</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
+        <v>123</v>
       </c>
       <c r="C24">
         <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>99</v>
+        <v>20</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>73</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>120</v>
+        <v>41</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="C25">
         <v>13</v>
       </c>
       <c r="D25" t="s">
-        <v>121</v>
+        <v>42</v>
       </c>
       <c r="E25">
         <v>9054619350</v>
@@ -1187,16 +1203,16 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="C26">
         <v>13</v>
       </c>
       <c r="D26" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="E26">
         <v>6474061810</v>
@@ -1204,58 +1220,58 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="5" t="s">
-        <v>88</v>
+        <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="C27">
         <v>17</v>
       </c>
       <c r="D27" t="s">
-        <v>90</v>
+        <v>11</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>91</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="5" t="s">
-        <v>92</v>
+        <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>93</v>
+        <v>14</v>
       </c>
       <c r="D28" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>94</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>122</v>
+        <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>123</v>
+        <v>44</v>
       </c>
       <c r="D29" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>124</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="D30" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="E30">
         <v>9054860203</v>
@@ -1263,7 +1279,7 @@
     </row>
     <row r="31" spans="1:5">
       <c r="B31" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="E31">
         <v>9059131216</v>
@@ -1271,62 +1287,62 @@
     </row>
     <row r="32" spans="1:5">
       <c r="B32" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="B33" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="B34" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="B35" t="s">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="D35" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>95</v>
+        <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>96</v>
+        <v>17</v>
       </c>
       <c r="D36" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>97</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="B37" t="s">
-        <v>98</v>
+        <v>19</v>
       </c>
       <c r="D37" t="s">
-        <v>99</v>
+        <v>20</v>
       </c>
       <c r="E37">
         <v>9058907919</v>
@@ -1334,13 +1350,13 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>102</v>
+        <v>23</v>
       </c>
       <c r="B38" t="s">
-        <v>101</v>
+        <v>22</v>
       </c>
       <c r="D38" t="s">
-        <v>99</v>
+        <v>20</v>
       </c>
       <c r="E38">
         <v>289232516</v>
@@ -1348,13 +1364,13 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>106</v>
+        <v>27</v>
       </c>
       <c r="D39" t="s">
-        <v>105</v>
+        <v>26</v>
       </c>
       <c r="E39">
         <v>4169535569</v>
@@ -1362,24 +1378,24 @@
     </row>
     <row r="40" spans="1:5" ht="16">
       <c r="A40" t="s">
-        <v>107</v>
+        <v>28</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>108</v>
+        <v>29</v>
       </c>
       <c r="C40">
         <v>21</v>
       </c>
       <c r="D40" t="s">
-        <v>109</v>
+        <v>30</v>
       </c>
       <c r="E40" t="s">
-        <v>110</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="B41" s="7" t="s">
-        <v>111</v>
+        <v>32</v>
       </c>
       <c r="E41">
         <v>4167233866</v>
@@ -1387,83 +1403,97 @@
     </row>
     <row r="42" spans="1:5">
       <c r="B42" s="7" t="s">
-        <v>112</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>116</v>
+        <v>37</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>113</v>
+        <v>34</v>
       </c>
       <c r="C43">
         <v>15</v>
       </c>
       <c r="D43" t="s">
-        <v>117</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="16">
       <c r="A44" t="s">
-        <v>114</v>
+        <v>35</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>115</v>
+        <v>36</v>
       </c>
       <c r="C44">
         <v>21</v>
       </c>
       <c r="D44" t="s">
-        <v>119</v>
+        <v>40</v>
       </c>
       <c r="E44" t="s">
-        <v>118</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
       <c r="C45">
         <v>14</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>85</v>
+        <v>6</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>86</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="19">
       <c r="A46" t="s">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>41</v>
+        <v>90</v>
       </c>
       <c r="D46" t="s">
-        <v>46</v>
+        <v>95</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="16">
       <c r="A47" s="11" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="D47" t="s">
+        <v>95</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="19">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="E47" s="11" t="s">
-        <v>44</v>
+      <c r="C48">
+        <v>13</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correcting volunteer's phone number
correcting volunteer's phone number
</commit_message>
<xml_diff>
--- a/campaign/VolunteerInformation.xlsx
+++ b/campaign/VolunteerInformation.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2140" yWindow="2460" windowWidth="21520" windowHeight="15400"/>
+    <workbookView xWindow="2145" yWindow="2460" windowWidth="21525" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -148,9 +148,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>(647) 822-7275</t>
-  </si>
-  <si>
     <t>Sheridan</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -426,13 +423,16 @@
   </si>
   <si>
     <t>David Suzuki Secondary School, Brampton</t>
+  </si>
+  <si>
+    <t>(647) 822-7274</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -546,6 +546,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -562,7 +630,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="7DE17D"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -840,53 +908,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="M48" sqref="M48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
         <v>65</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>66</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>67</v>
       </c>
-      <c r="D1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>68</v>
-      </c>
-      <c r="B2" t="s">
-        <v>69</v>
       </c>
       <c r="C2">
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E2" s="2">
         <v>6472445427</v>
@@ -895,29 +963,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C3">
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
         <v>74</v>
-      </c>
-      <c r="B4" t="s">
-        <v>75</v>
       </c>
       <c r="C4">
         <v>17</v>
@@ -926,224 +994,224 @@
         <v>4165621762</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
         <v>76</v>
-      </c>
-      <c r="B5" t="s">
-        <v>77</v>
       </c>
       <c r="C5">
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="C6">
         <v>14</v>
       </c>
       <c r="D6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>80</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
+      <c r="B7" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="C7">
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E7" s="2">
         <v>6478600426</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" t="s">
         <v>83</v>
-      </c>
-      <c r="B8" t="s">
-        <v>84</v>
       </c>
       <c r="C8">
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E8" s="2">
         <v>6477678445</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" t="s">
         <v>86</v>
-      </c>
-      <c r="B9" t="s">
-        <v>87</v>
       </c>
       <c r="C9">
         <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C10">
         <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E10" s="2">
         <v>4166711521</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" t="s">
         <v>97</v>
-      </c>
-      <c r="B11" t="s">
-        <v>98</v>
       </c>
       <c r="C11">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E11" s="2">
         <v>6478295824</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" t="s">
         <v>99</v>
-      </c>
-      <c r="B12" t="s">
-        <v>100</v>
       </c>
       <c r="C12">
         <v>14</v>
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C13">
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E13" s="2">
         <v>9056731538</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C14">
         <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>105</v>
+      </c>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>106</v>
       </c>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="B16" t="s">
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="B17" s="1" t="s">
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>108</v>
       </c>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="B18" t="s">
-        <v>109</v>
-      </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>111</v>
       </c>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="B21" t="s">
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>112</v>
       </c>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" t="s">
+      <c r="B22" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="C22">
         <v>16</v>
@@ -1152,27 +1220,27 @@
         <v>20</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" t="s">
         <v>119</v>
-      </c>
-      <c r="B23" t="s">
-        <v>120</v>
       </c>
       <c r="C23">
         <v>14</v>
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C24">
         <v>16</v>
@@ -1181,12 +1249,12 @@
         <v>20</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>0</v>
@@ -1195,15 +1263,15 @@
         <v>13</v>
       </c>
       <c r="D25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E25">
         <v>9054619350</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B26" t="s">
         <v>1</v>
@@ -1212,13 +1280,13 @@
         <v>13</v>
       </c>
       <c r="D26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E26">
         <v>6474061810</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>9</v>
       </c>
@@ -1235,7 +1303,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>13</v>
       </c>
@@ -1243,84 +1311,84 @@
         <v>14</v>
       </c>
       <c r="D28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" t="s">
         <v>43</v>
       </c>
-      <c r="B29" t="s">
+      <c r="D29" t="s">
+        <v>71</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D29" t="s">
-        <v>72</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" t="s">
         <v>49</v>
-      </c>
-      <c r="D30" t="s">
-        <v>50</v>
       </c>
       <c r="E30">
         <v>9054860203</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E31">
         <v>9059131216</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E32" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="B33" t="s">
-        <v>61</v>
-      </c>
       <c r="E33" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
-      <c r="B34" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" t="s">
         <v>51</v>
       </c>
-      <c r="B35" t="s">
+      <c r="D35" t="s">
         <v>52</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>16</v>
       </c>
@@ -1328,13 +1396,13 @@
         <v>17</v>
       </c>
       <c r="D36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>21</v>
       </c>
@@ -1348,7 +1416,7 @@
         <v>9058907919</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>23</v>
       </c>
@@ -1362,7 +1430,7 @@
         <v>289232516</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -1376,7 +1444,7 @@
         <v>4169535569</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="16">
+    <row r="40" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>28</v>
       </c>
@@ -1393,7 +1461,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41" s="7" t="s">
         <v>32</v>
       </c>
@@ -1401,12 +1469,12 @@
         <v>4167233866</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B42" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -1420,7 +1488,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="16">
+    <row r="44" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>35</v>
       </c>
@@ -1431,13 +1499,13 @@
         <v>21</v>
       </c>
       <c r="D44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E44" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>5</v>
       </c>
@@ -1454,46 +1522,46 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="19">
+    <row r="46" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>88</v>
+      </c>
+      <c r="B46" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="D46" t="s">
+        <v>94</v>
+      </c>
+      <c r="E46" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D46" t="s">
-        <v>95</v>
-      </c>
-      <c r="E46" s="10" t="s">
+    </row>
+    <row r="47" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A47" s="11" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" ht="16">
-      <c r="A47" s="11" t="s">
+      <c r="B47" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D47" t="s">
+        <v>94</v>
+      </c>
+      <c r="E47" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="B47" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D47" t="s">
-        <v>95</v>
-      </c>
-      <c r="E47" s="11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="19">
+    </row>
+    <row r="48" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C48">
         <v>13</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1524,12 +1592,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1541,12 +1609,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
moving flyers  and election signs to different sub folders
moving flyers  and election signs to different sub folders
</commit_message>
<xml_diff>
--- a/campaign/VolunteerInformation.xlsx
+++ b/campaign/VolunteerInformation.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2145" yWindow="2460" windowWidth="21525" windowHeight="13740"/>
+    <workbookView xWindow="2145" yWindow="2460" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -310,9 +310,6 @@
     <t>aliturablotia@gmail.com</t>
   </si>
   <si>
-    <t>647-997-085</t>
-  </si>
-  <si>
     <t>Paul Konieczny</t>
   </si>
   <si>
@@ -432,13 +429,16 @@
   </si>
   <si>
     <t>905 612 8353</t>
+  </si>
+  <si>
+    <t>647-997-0852</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -636,7 +636,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="7DE17D"/>
+        <a:sysClr val="window" lastClr="78DC78"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -703,7 +703,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -738,7 +737,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -914,14 +912,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.28515625" bestFit="1" customWidth="1"/>
@@ -929,7 +927,7 @@
     <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -943,13 +941,13 @@
         <v>69</v>
       </c>
       <c r="E1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -969,7 +967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -983,10 +981,10 @@
         <v>70</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>72</v>
       </c>
@@ -1000,7 +998,7 @@
         <v>4165621762</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>74</v>
       </c>
@@ -1011,13 +1009,13 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -1031,10 +1029,10 @@
         <v>78</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -1045,13 +1043,13 @@
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E7" s="2">
         <v>6478600426</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>81</v>
       </c>
@@ -1068,7 +1066,7 @@
         <v>6477678445</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>84</v>
       </c>
@@ -1085,12 +1083,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>86</v>
       </c>
       <c r="B10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C10">
         <v>21</v>
@@ -1102,12 +1100,12 @@
         <v>4166711521</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" t="s">
         <v>95</v>
-      </c>
-      <c r="B11" t="s">
-        <v>96</v>
       </c>
       <c r="C11">
         <v>14</v>
@@ -1119,110 +1117,110 @@
         <v>6478295824</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" t="s">
         <v>97</v>
-      </c>
-      <c r="B12" t="s">
-        <v>98</v>
       </c>
       <c r="C12">
         <v>14</v>
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C13">
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E13" s="2">
         <v>9056731538</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C14">
         <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="B15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C15">
         <v>15</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="B16" t="s">
+        <v>104</v>
+      </c>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="B17" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="B18" t="s">
         <v>106</v>
       </c>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>107</v>
-      </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="B20" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="B21" t="s">
         <v>109</v>
       </c>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
         <v>110</v>
       </c>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B22" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="C22">
         <v>16</v>
@@ -1231,27 +1229,27 @@
         <v>20</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" t="s">
         <v>117</v>
-      </c>
-      <c r="B23" t="s">
-        <v>118</v>
       </c>
       <c r="C23">
         <v>14</v>
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C24">
         <v>16</v>
@@ -1260,10 +1258,10 @@
         <v>20</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -1280,7 +1278,7 @@
         <v>9054619350</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -1297,7 +1295,7 @@
         <v>6474061810</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="5" t="s">
         <v>9</v>
       </c>
@@ -1314,7 +1312,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="5" t="s">
         <v>13</v>
       </c>
@@ -1328,7 +1326,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -1342,7 +1340,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -1352,11 +1350,8 @@
       <c r="D30" t="s">
         <v>48</v>
       </c>
-      <c r="E30">
-        <v>9054860203</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:5">
       <c r="B31" t="s">
         <v>54</v>
       </c>
@@ -1364,7 +1359,7 @@
         <v>9059131216</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="B32" t="s">
         <v>55</v>
       </c>
@@ -1372,7 +1367,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="B33" t="s">
         <v>59</v>
       </c>
@@ -1380,12 +1375,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="B34" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>49</v>
       </c>
@@ -1399,7 +1394,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>16</v>
       </c>
@@ -1413,7 +1408,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>21</v>
       </c>
@@ -1427,7 +1422,7 @@
         <v>9058907919</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>23</v>
       </c>
@@ -1441,7 +1436,7 @@
         <v>289232516</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -1455,7 +1450,7 @@
         <v>4169535569</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="17.25">
       <c r="A40" t="s">
         <v>28</v>
       </c>
@@ -1472,7 +1467,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="B41" s="7" t="s">
         <v>32</v>
       </c>
@@ -1480,12 +1475,12 @@
         <v>4167233866</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="B42" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -1499,7 +1494,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="17.25">
       <c r="A44" t="s">
         <v>35</v>
       </c>
@@ -1513,10 +1508,10 @@
         <v>39</v>
       </c>
       <c r="E44" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>5</v>
       </c>
@@ -1533,7 +1528,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="18.75">
       <c r="A46" t="s">
         <v>87</v>
       </c>
@@ -1541,27 +1536,27 @@
         <v>88</v>
       </c>
       <c r="D46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E46" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="16.5">
+      <c r="A47" s="11" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="11" t="s">
+      <c r="B47" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D47" t="s">
+        <v>92</v>
+      </c>
+      <c r="E47" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="B47" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D47" t="s">
-        <v>93</v>
-      </c>
-      <c r="E47" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:5" ht="18.75">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -1572,10 +1567,10 @@
         <v>13</v>
       </c>
       <c r="D48" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="E48" t="s">
         <v>127</v>
-      </c>
-      <c r="E48" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1606,12 +1601,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1623,12 +1618,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
updating volunteer info, Chinese release and schedule
updating volunteer info, Chinese release and schedule
</commit_message>
<xml_diff>
--- a/campaign/VolunteerInformation.xlsx
+++ b/campaign/VolunteerInformation.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="2145" yWindow="2460" windowWidth="20730" windowHeight="11760"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="135">
   <si>
     <t>jetaix01@yahoo.ca</t>
   </si>
@@ -441,13 +441,19 @@
   </si>
   <si>
     <t>(437) 580-0905 / (905) 205-0304</t>
+  </si>
+  <si>
+    <t>aritankovic@gmail.com</t>
+  </si>
+  <si>
+    <t>Armin Tankovic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -645,7 +651,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="78DC78"/>
+        <a:sysClr val="window" lastClr="7DE17D"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -712,6 +718,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -746,6 +753,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -921,14 +929,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.28515625" bestFit="1" customWidth="1"/>
@@ -936,7 +944,7 @@
     <col min="5" max="5" width="28.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -956,7 +964,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -976,7 +984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -993,7 +1001,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>72</v>
       </c>
@@ -1007,7 +1015,7 @@
         <v>4165621762</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>74</v>
       </c>
@@ -1024,7 +1032,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -1041,7 +1049,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -1058,7 +1066,7 @@
         <v>6478600426</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>81</v>
       </c>
@@ -1075,7 +1083,7 @@
         <v>6477678445</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>84</v>
       </c>
@@ -1092,7 +1100,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>86</v>
       </c>
@@ -1109,7 +1117,7 @@
         <v>4166711521</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>94</v>
       </c>
@@ -1126,7 +1134,7 @@
         <v>6478295824</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>96</v>
       </c>
@@ -1138,7 +1146,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>121</v>
       </c>
@@ -1155,7 +1163,7 @@
         <v>9056731538</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>123</v>
       </c>
@@ -1172,7 +1180,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>103</v>
       </c>
@@ -1183,25 +1191,25 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>104</v>
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>105</v>
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>106</v>
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -1212,19 +1220,19 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>108</v>
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>109</v>
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>110</v>
       </c>
@@ -1241,7 +1249,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>116</v>
       </c>
@@ -1253,7 +1261,7 @@
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>118</v>
       </c>
@@ -1270,7 +1278,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -1287,7 +1295,7 @@
         <v>9054619350</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -1304,7 +1312,7 @@
         <v>6474061810</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>9</v>
       </c>
@@ -1321,7 +1329,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>13</v>
       </c>
@@ -1335,7 +1343,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -1349,7 +1357,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -1363,7 +1371,7 @@
         <v>9054860232</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>54</v>
       </c>
@@ -1371,7 +1379,7 @@
         <v>9059131216</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>55</v>
       </c>
@@ -1379,7 +1387,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>59</v>
       </c>
@@ -1387,12 +1395,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>49</v>
       </c>
@@ -1406,7 +1414,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>16</v>
       </c>
@@ -1420,7 +1428,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>21</v>
       </c>
@@ -1434,7 +1442,7 @@
         <v>9058907919</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>23</v>
       </c>
@@ -1448,7 +1456,7 @@
         <v>289232516</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -1462,7 +1470,7 @@
         <v>4169535569</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="17.25">
+    <row r="40" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>28</v>
       </c>
@@ -1479,7 +1487,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41" s="7" t="s">
         <v>32</v>
       </c>
@@ -1487,12 +1495,12 @@
         <v>4167233866</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B42" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -1506,7 +1514,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="17.25">
+    <row r="44" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>35</v>
       </c>
@@ -1523,7 +1531,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>5</v>
       </c>
@@ -1540,7 +1548,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="18.75">
+    <row r="46" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>87</v>
       </c>
@@ -1554,7 +1562,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="16.5">
+    <row r="47" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>89</v>
       </c>
@@ -1568,7 +1576,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="18.75">
+    <row r="48" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -1585,7 +1593,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>130</v>
       </c>
@@ -1600,6 +1608,20 @@
       </c>
       <c r="E49" t="s">
         <v>132</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>134</v>
+      </c>
+      <c r="B50" t="s">
+        <v>133</v>
+      </c>
+      <c r="D50" t="s">
+        <v>70</v>
+      </c>
+      <c r="E50">
+        <v>6478227275</v>
       </c>
     </row>
   </sheetData>
@@ -1630,12 +1652,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1647,12 +1669,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Updated volunteer list on excel
</commit_message>
<xml_diff>
--- a/campaign/VolunteerInformation.xlsx
+++ b/campaign/VolunteerInformation.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2145" yWindow="2460" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="500" yWindow="-20" windowWidth="13880" windowHeight="15220"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,229 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="148">
+  <si>
+    <t>Zakira</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>karbaryz@gmail.com</t>
+  </si>
+  <si>
+    <t>dezaya.joseph@hotmail.com </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>hspathan13@gmail.com</t>
+  </si>
+  <si>
+    <t>David Leeder Middle School</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nasra Nadeem </t>
+  </si>
+  <si>
+    <t>nasra.nadeem@hotmail.com</t>
+  </si>
+  <si>
+    <t>Uswa Zahoor</t>
+  </si>
+  <si>
+    <t>uswa.zahoor@hotmail.ca</t>
+  </si>
+  <si>
+    <t>Glenforest Secondary School</t>
+  </si>
+  <si>
+    <t>Michael Jackman</t>
+  </si>
+  <si>
+    <t>michaelericjackman@gmail.com</t>
+  </si>
+  <si>
+    <t>Ayesha Faizi</t>
+  </si>
+  <si>
+    <t>Ali Turab Lotia</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>aliturablotia@gmail.com</t>
+  </si>
+  <si>
+    <t>Paul Konieczny</t>
+  </si>
+  <si>
+    <t>647-217-2793</t>
+  </si>
+  <si>
+    <t>pkonieczny@rogers.com</t>
+  </si>
+  <si>
+    <t>UTM</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ayesha.f13@gmail.com</t>
+  </si>
+  <si>
+    <t>Vivian Li</t>
+  </si>
+  <si>
+    <t>vivi881121@gmail.com</t>
+  </si>
+  <si>
+    <t>Diya</t>
+  </si>
+  <si>
+    <t>diyakamath@yahoo.ca</t>
+  </si>
+  <si>
+    <t>Stephen Lewis Secondary</t>
+  </si>
+  <si>
+    <t>David Suzuki Secondary</t>
+  </si>
+  <si>
+    <t>Contact Number</t>
+  </si>
+  <si>
+    <t>annie.195@hotmail.com</t>
+  </si>
+  <si>
+    <t>fatehhayer1999@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> hawkstar@live.ca</t>
+  </si>
+  <si>
+    <t>mikayla_december@outlook.com</t>
+  </si>
+  <si>
+    <t>imranshaista@hotmail.com</t>
+  </si>
+  <si>
+    <t>sundaram_balas@yahoo.ca</t>
+  </si>
+  <si>
+    <t>taimoorgul98@gmail.com</t>
+  </si>
+  <si>
+    <t>mmdj360@gmail.com</t>
+  </si>
+  <si>
+    <t>Xenwraith@gmail.com</t>
+  </si>
+  <si>
+    <t>Jordan Gray</t>
+  </si>
+  <si>
+    <t>jordancgray@hotmail.com</t>
+  </si>
+  <si>
+    <t>(647) 233-4244</t>
+  </si>
+  <si>
+    <t>416-737-7706 / 647-767-9601</t>
+  </si>
+  <si>
+    <t>416-738-3281</t>
+  </si>
+  <si>
+    <t>Drive</t>
+  </si>
+  <si>
+    <t>Syed Abdullah Hussain</t>
+  </si>
+  <si>
+    <t>abd_pisces@live.com</t>
+  </si>
+  <si>
+    <t>Dylan Leonard</t>
+  </si>
+  <si>
+    <t>647 783 6844</t>
+  </si>
+  <si>
+    <t>dy2_leonard@hotmail.com</t>
+  </si>
+  <si>
+    <t>Anisha Akhtar</t>
+  </si>
+  <si>
+    <t>York University</t>
+  </si>
+  <si>
+    <t>Fateh Hayer</t>
+  </si>
+  <si>
+    <t>David Suzuki Secondary School, Brampton</t>
+  </si>
+  <si>
+    <t>(647) 822-7274</t>
+  </si>
+  <si>
+    <t>Ascension of Our Lord</t>
+  </si>
+  <si>
+    <t>905 405 9413</t>
+  </si>
+  <si>
+    <t>905 612 8353</t>
+  </si>
+  <si>
+    <t>647-997-0852</t>
+  </si>
+  <si>
+    <t>Vigil Vincent</t>
+  </si>
+  <si>
+    <t>vigiljoe24@gmail.com</t>
+  </si>
+  <si>
+    <t>(437) 580-0905 / (905) 205-0304</t>
+  </si>
+  <si>
+    <t>aritankovic@gmail.com</t>
+  </si>
+  <si>
+    <t>Armin Tankovic</t>
+  </si>
+  <si>
+    <t>Dezaya Joseph</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brandon Prakash</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pabdeep</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lincoln Alexander Secondary School. </t>
+  </si>
+  <si>
+    <t>brandon.prakash@hotmail.com</t>
+  </si>
+  <si>
+    <t> 905 678 6526</t>
+  </si>
+  <si>
+    <t>905 956 1163</t>
+  </si>
+  <si>
+    <t>Lincoln Alexander Secondary School. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>panesar.panesar@gmail.com</t>
+  </si>
+  <si>
+    <t>St. Joseph</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
   <si>
     <t>jetaix01@yahoo.ca</t>
   </si>
@@ -271,189 +493,13 @@
   </si>
   <si>
     <t>Humza Pathan</t>
-  </si>
-  <si>
-    <t>hspathan13@gmail.com</t>
-  </si>
-  <si>
-    <t>David Leeder Middle School</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nasra Nadeem </t>
-  </si>
-  <si>
-    <t>nasra.nadeem@hotmail.com</t>
-  </si>
-  <si>
-    <t>Uswa Zahoor</t>
-  </si>
-  <si>
-    <t>uswa.zahoor@hotmail.ca</t>
-  </si>
-  <si>
-    <t>Glenforest Secondary School</t>
-  </si>
-  <si>
-    <t>Michael Jackman</t>
-  </si>
-  <si>
-    <t>michaelericjackman@gmail.com</t>
-  </si>
-  <si>
-    <t>Ayesha Faizi</t>
-  </si>
-  <si>
-    <t>Ali Turab Lotia</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>aliturablotia@gmail.com</t>
-  </si>
-  <si>
-    <t>Paul Konieczny</t>
-  </si>
-  <si>
-    <t>647-217-2793</t>
-  </si>
-  <si>
-    <t>pkonieczny@rogers.com</t>
-  </si>
-  <si>
-    <t>UTM</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ayesha.f13@gmail.com</t>
-  </si>
-  <si>
-    <t>Vivian Li</t>
-  </si>
-  <si>
-    <t>vivi881121@gmail.com</t>
-  </si>
-  <si>
-    <t>Diya</t>
-  </si>
-  <si>
-    <t>diyakamath@yahoo.ca</t>
-  </si>
-  <si>
-    <t>Stephen Lewis Secondary</t>
-  </si>
-  <si>
-    <t>David Suzuki Secondary</t>
-  </si>
-  <si>
-    <t>Contact Number</t>
-  </si>
-  <si>
-    <t>annie.195@hotmail.com</t>
-  </si>
-  <si>
-    <t>fatehhayer1999@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> hawkstar@live.ca</t>
-  </si>
-  <si>
-    <t>mikayla_december@outlook.com</t>
-  </si>
-  <si>
-    <t>imranshaista@hotmail.com</t>
-  </si>
-  <si>
-    <t>sundaram_balas@yahoo.ca</t>
-  </si>
-  <si>
-    <t>taimoorgul98@gmail.com</t>
-  </si>
-  <si>
-    <t>mmdj360@gmail.com</t>
-  </si>
-  <si>
-    <t>Xenwraith@gmail.com</t>
-  </si>
-  <si>
-    <t>Jordan Gray</t>
-  </si>
-  <si>
-    <t>jordancgray@hotmail.com</t>
-  </si>
-  <si>
-    <t>(647) 233-4244</t>
-  </si>
-  <si>
-    <t>416-737-7706 / 647-767-9601</t>
-  </si>
-  <si>
-    <t>416-738-3281</t>
-  </si>
-  <si>
-    <t>Drive</t>
-  </si>
-  <si>
-    <t>Syed Abdullah Hussain</t>
-  </si>
-  <si>
-    <t>abd_pisces@live.com</t>
-  </si>
-  <si>
-    <t>Dylan Leonard</t>
-  </si>
-  <si>
-    <t>647 783 6844</t>
-  </si>
-  <si>
-    <t>dy2_leonard@hotmail.com</t>
-  </si>
-  <si>
-    <t>Anisha Akhtar</t>
-  </si>
-  <si>
-    <t>York University</t>
-  </si>
-  <si>
-    <t>Fateh Hayer</t>
-  </si>
-  <si>
-    <t>David Suzuki Secondary School, Brampton</t>
-  </si>
-  <si>
-    <t>(647) 822-7274</t>
-  </si>
-  <si>
-    <t>Ascension of Our Lord</t>
-  </si>
-  <si>
-    <t>905 405 9413</t>
-  </si>
-  <si>
-    <t>905 612 8353</t>
-  </si>
-  <si>
-    <t>647-997-0852</t>
-  </si>
-  <si>
-    <t>Vigil Vincent</t>
-  </si>
-  <si>
-    <t>vigiljoe24@gmail.com</t>
-  </si>
-  <si>
-    <t>(437) 580-0905 / (905) 205-0304</t>
-  </si>
-  <si>
-    <t>aritankovic@gmail.com</t>
-  </si>
-  <si>
-    <t>Armin Tankovic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -567,74 +613,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -651,7 +629,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="7DE17D"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -929,53 +907,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>134</v>
       </c>
       <c r="B1" t="s">
-        <v>64</v>
+        <v>135</v>
       </c>
       <c r="C1" t="s">
-        <v>65</v>
+        <v>136</v>
       </c>
       <c r="D1" t="s">
-        <v>69</v>
+        <v>140</v>
       </c>
       <c r="E1" t="s">
-        <v>100</v>
+        <v>26</v>
       </c>
       <c r="F1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>137</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>138</v>
       </c>
       <c r="C2">
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>141</v>
       </c>
       <c r="E2" s="2">
         <v>6472445427</v>
@@ -984,29 +962,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>139</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>142</v>
       </c>
       <c r="C3">
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>141</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>143</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>144</v>
       </c>
       <c r="C4">
         <v>17</v>
@@ -1015,613 +993,669 @@
         <v>4165621762</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>145</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>146</v>
       </c>
       <c r="C5">
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>147</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>77</v>
+        <v>3</v>
       </c>
       <c r="C6">
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>99</v>
+        <v>25</v>
       </c>
       <c r="E7" s="2">
         <v>6478600426</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>81</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="E8" s="2">
         <v>6477678445</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="C9">
         <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
+        <v>141</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>93</v>
+        <v>19</v>
       </c>
       <c r="C10">
         <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>70</v>
+        <v>141</v>
       </c>
       <c r="E10" s="2">
         <v>4166711521</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>21</v>
       </c>
       <c r="C11">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="E11" s="2">
         <v>6478295824</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>96</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>97</v>
+        <v>23</v>
       </c>
       <c r="C12">
         <v>14</v>
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>121</v>
+        <v>47</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>101</v>
+        <v>27</v>
       </c>
       <c r="C13">
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>122</v>
+        <v>48</v>
       </c>
       <c r="E13" s="2">
         <v>9056731538</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>123</v>
+        <v>49</v>
       </c>
       <c r="B14" t="s">
-        <v>102</v>
+        <v>28</v>
       </c>
       <c r="C14">
         <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>124</v>
+        <v>50</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="B15" t="s">
-        <v>103</v>
+        <v>29</v>
       </c>
       <c r="C15">
         <v>15</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="B16" t="s">
-        <v>104</v>
+        <v>30</v>
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="B17" s="1" t="s">
-        <v>105</v>
+        <v>31</v>
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="B18" t="s">
-        <v>106</v>
+        <v>32</v>
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>2</v>
+        <v>73</v>
       </c>
       <c r="B19" t="s">
-        <v>107</v>
+        <v>33</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="B20" s="1" t="s">
-        <v>108</v>
+        <v>34</v>
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="B21" t="s">
-        <v>109</v>
+        <v>35</v>
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>110</v>
+        <v>36</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>111</v>
+        <v>37</v>
       </c>
       <c r="C22">
         <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>116</v>
+        <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>117</v>
+        <v>43</v>
       </c>
       <c r="C23">
         <v>14</v>
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>118</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>120</v>
+        <v>46</v>
       </c>
       <c r="C24">
         <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="C25">
         <v>13</v>
       </c>
       <c r="D25" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="E25">
         <v>9054619350</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>127</v>
       </c>
       <c r="B26" t="s">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="C26">
         <v>13</v>
       </c>
       <c r="D26" t="s">
-        <v>57</v>
+        <v>128</v>
       </c>
       <c r="E26">
         <v>6474061810</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="5" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="C27">
         <v>17</v>
       </c>
       <c r="D27" t="s">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="5" t="s">
-        <v>13</v>
+        <v>84</v>
       </c>
       <c r="B28" t="s">
-        <v>14</v>
+        <v>85</v>
       </c>
       <c r="D28" t="s">
-        <v>70</v>
+        <v>141</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>113</v>
       </c>
       <c r="B29" t="s">
-        <v>43</v>
+        <v>114</v>
       </c>
       <c r="D29" t="s">
-        <v>70</v>
+        <v>141</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>124</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>47</v>
+        <v>118</v>
       </c>
       <c r="D30" t="s">
-        <v>48</v>
+        <v>119</v>
       </c>
       <c r="E30">
         <v>9054860232</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="B31" t="s">
-        <v>54</v>
+        <v>125</v>
       </c>
       <c r="E31">
         <v>9059131216</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="B32" t="s">
-        <v>55</v>
+        <v>126</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="B33" t="s">
-        <v>59</v>
+        <v>130</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="B34" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>49</v>
+        <v>120</v>
       </c>
       <c r="B35" t="s">
-        <v>50</v>
+        <v>121</v>
       </c>
       <c r="D35" t="s">
-        <v>51</v>
+        <v>122</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="B36" t="s">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="D36" t="s">
-        <v>70</v>
+        <v>141</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>21</v>
+        <v>92</v>
       </c>
       <c r="B37" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
       <c r="D37" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="E37">
         <v>9058907919</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="B38" t="s">
-        <v>22</v>
+        <v>93</v>
       </c>
       <c r="D38" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="E38">
         <v>289232516</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>25</v>
+        <v>96</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>27</v>
+        <v>98</v>
       </c>
       <c r="D39" t="s">
-        <v>26</v>
+        <v>97</v>
       </c>
       <c r="E39">
         <v>4169535569</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="16">
       <c r="A40" t="s">
-        <v>28</v>
+        <v>99</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>29</v>
+        <v>100</v>
       </c>
       <c r="C40">
         <v>21</v>
       </c>
       <c r="D40" t="s">
-        <v>30</v>
+        <v>101</v>
       </c>
       <c r="E40" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="B41" s="7" t="s">
-        <v>32</v>
+        <v>103</v>
       </c>
       <c r="E41">
         <v>4167233866</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="B42" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>37</v>
+        <v>108</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>34</v>
+        <v>105</v>
       </c>
       <c r="C43">
         <v>15</v>
       </c>
       <c r="D43" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="16">
       <c r="A44" t="s">
-        <v>35</v>
+        <v>106</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>36</v>
+        <v>107</v>
       </c>
       <c r="C44">
         <v>21</v>
       </c>
       <c r="D44" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="E44" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>5</v>
+        <v>76</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
       <c r="C45">
         <v>14</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>6</v>
+        <v>77</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="19">
       <c r="A46" t="s">
-        <v>87</v>
+        <v>13</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>88</v>
+        <v>14</v>
       </c>
       <c r="D46" t="s">
-        <v>92</v>
+        <v>18</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="16">
       <c r="A47" s="11" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="D47" t="s">
-        <v>92</v>
+        <v>18</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="19">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>117</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>45</v>
+        <v>116</v>
       </c>
       <c r="C48">
         <v>13</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>126</v>
+        <v>52</v>
       </c>
       <c r="E48" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>130</v>
+        <v>56</v>
       </c>
       <c r="B49" t="s">
-        <v>131</v>
+        <v>57</v>
       </c>
       <c r="C49">
         <v>17</v>
       </c>
       <c r="D49" t="s">
-        <v>126</v>
+        <v>52</v>
       </c>
       <c r="E49" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>134</v>
+        <v>60</v>
       </c>
       <c r="B50" t="s">
-        <v>133</v>
+        <v>59</v>
       </c>
       <c r="D50" t="s">
-        <v>70</v>
+        <v>141</v>
       </c>
       <c r="E50">
         <v>6478227275</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="19">
+      <c r="A51" t="s">
+        <v>61</v>
+      </c>
+      <c r="B51" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E51" s="10">
+        <v>6476336597</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="19">
+      <c r="A52" t="s">
+        <v>62</v>
+      </c>
+      <c r="B52" t="s">
+        <v>65</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="19">
+      <c r="A53" t="s">
+        <v>63</v>
+      </c>
+      <c r="B53" t="s">
+        <v>69</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="19">
+      <c r="A54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E54" s="10">
+        <v>6473626012</v>
       </c>
     </row>
   </sheetData>
@@ -1641,8 +1675,10 @@
     <hyperlink ref="B43" r:id="rId12"/>
     <hyperlink ref="B46" r:id="rId13"/>
     <hyperlink ref="B47" r:id="rId14"/>
+    <hyperlink ref="B54" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1652,12 +1688,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1669,12 +1705,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
removing badly named poll phone files
removing badly named poll phone files
</commit_message>
<xml_diff>
--- a/campaign/VolunteerInformation.xlsx
+++ b/campaign/VolunteerInformation.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="154">
   <si>
     <t>Zakira</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -499,6 +499,18 @@
   </si>
   <si>
     <t>(647) 280-2192</t>
+  </si>
+  <si>
+    <t>6477195000 / 9054059413</t>
+  </si>
+  <si>
+    <t>Faraz</t>
+  </si>
+  <si>
+    <t>faraz_tahir@hotmail.com</t>
+  </si>
+  <si>
+    <t>Phone Canvasser?</t>
   </si>
 </sst>
 </file>
@@ -982,10 +994,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" topLeftCell="D34" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1708,8 +1720,8 @@
       <c r="D53" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E53">
-        <v>6477195000</v>
+      <c r="E53" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="18.75">
@@ -1724,6 +1736,20 @@
       </c>
       <c r="E54" t="s">
         <v>149</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="18.75">
+      <c r="A55" t="s">
+        <v>151</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="E55">
+        <v>6475206843</v>
       </c>
     </row>
   </sheetData>
@@ -1744,6 +1770,7 @@
     <hyperlink ref="B43" r:id="rId13"/>
     <hyperlink ref="B50" r:id="rId14"/>
     <hyperlink ref="B53" r:id="rId15"/>
+    <hyperlink ref="B55" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
edited one contact info
</commit_message>
<xml_diff>
--- a/campaign/VolunteerInformation.xlsx
+++ b/campaign/VolunteerInformation.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="495" yWindow="-15" windowWidth="13875" windowHeight="11760"/>
+    <workbookView xWindow="-40" yWindow="-80" windowWidth="21340" windowHeight="13300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,246 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="150">
-  <si>
-    <t>Zakira</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>karbaryz@gmail.com</t>
-  </si>
-  <si>
-    <t>dezaya.joseph@hotmail.com </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>hspathan13@gmail.com</t>
-  </si>
-  <si>
-    <t>David Leeder Middle School</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nasra Nadeem </t>
-  </si>
-  <si>
-    <t>nasra.nadeem@hotmail.com</t>
-  </si>
-  <si>
-    <t>Uswa Zahoor</t>
-  </si>
-  <si>
-    <t>uswa.zahoor@hotmail.ca</t>
-  </si>
-  <si>
-    <t>Glenforest Secondary School</t>
-  </si>
-  <si>
-    <t>Michael Jackman</t>
-  </si>
-  <si>
-    <t>michaelericjackman@gmail.com</t>
-  </si>
-  <si>
-    <t>Ayesha Faizi</t>
-  </si>
-  <si>
-    <t>Ali Turab Lotia</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>aliturablotia@gmail.com</t>
-  </si>
-  <si>
-    <t>Paul Konieczny</t>
-  </si>
-  <si>
-    <t>647-217-2793</t>
-  </si>
-  <si>
-    <t>pkonieczny@rogers.com</t>
-  </si>
-  <si>
-    <t>UTM</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ayesha.f13@gmail.com</t>
-  </si>
-  <si>
-    <t>Vivian Li</t>
-  </si>
-  <si>
-    <t>vivi881121@gmail.com</t>
-  </si>
-  <si>
-    <t>Diya</t>
-  </si>
-  <si>
-    <t>diyakamath@yahoo.ca</t>
-  </si>
-  <si>
-    <t>Stephen Lewis Secondary</t>
-  </si>
-  <si>
-    <t>David Suzuki Secondary</t>
-  </si>
-  <si>
-    <t>Contact Number</t>
-  </si>
-  <si>
-    <t>annie.195@hotmail.com</t>
-  </si>
-  <si>
-    <t>fatehhayer1999@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> hawkstar@live.ca</t>
-  </si>
-  <si>
-    <t>mikayla_december@outlook.com</t>
-  </si>
-  <si>
-    <t>imranshaista@hotmail.com</t>
-  </si>
-  <si>
-    <t>sundaram_balas@yahoo.ca</t>
-  </si>
-  <si>
-    <t>taimoorgul98@gmail.com</t>
-  </si>
-  <si>
-    <t>mmdj360@gmail.com</t>
-  </si>
-  <si>
-    <t>Xenwraith@gmail.com</t>
-  </si>
-  <si>
-    <t>416-737-7706 / 647-767-9601</t>
-  </si>
-  <si>
-    <t>416-738-3281</t>
-  </si>
-  <si>
-    <t>Drive</t>
-  </si>
-  <si>
-    <t>Syed Abdullah Hussain</t>
-  </si>
-  <si>
-    <t>abd_pisces@live.com</t>
-  </si>
-  <si>
-    <t>Anisha Akhtar</t>
-  </si>
-  <si>
-    <t>York University</t>
-  </si>
-  <si>
-    <t>Fateh Hayer</t>
-  </si>
-  <si>
-    <t>David Suzuki Secondary School, Brampton</t>
-  </si>
-  <si>
-    <t>(647) 822-7274</t>
-  </si>
-  <si>
-    <t>Ascension of Our Lord</t>
-  </si>
-  <si>
-    <t>905 405 9413</t>
-  </si>
-  <si>
-    <t>905 612 8353</t>
-  </si>
-  <si>
-    <t>647-997-0852</t>
-  </si>
-  <si>
-    <t>Vigil Vincent</t>
-  </si>
-  <si>
-    <t>vigiljoe24@gmail.com</t>
-  </si>
-  <si>
-    <t>(437) 580-0905 / (905) 205-0304</t>
-  </si>
-  <si>
-    <t>aritankovic@gmail.com</t>
-  </si>
-  <si>
-    <t>Armin Tankovic</t>
-  </si>
-  <si>
-    <t>Dezaya Joseph</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Brandon Prakash</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pabdeep</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lincoln Alexander Secondary School. </t>
-  </si>
-  <si>
-    <t>brandon.prakash@hotmail.com</t>
-  </si>
-  <si>
-    <t> 905 678 6526</t>
-  </si>
-  <si>
-    <t>905 956 1163</t>
-  </si>
-  <si>
-    <t>Lincoln Alexander Secondary School. </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>panesar.panesar@gmail.com</t>
-  </si>
-  <si>
-    <t>St. Joseph</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>jetaix01@yahoo.ca</t>
-  </si>
-  <si>
-    <t>fawaddv@gmail.com</t>
-  </si>
-  <si>
-    <t>Taimoor</t>
-  </si>
-  <si>
-    <t>647-300-0101 / 647 960 1002</t>
-  </si>
-  <si>
-    <t>tanvi1111@hotmail.com</t>
-  </si>
-  <si>
-    <t>Tanvi Mehta</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gordon Graydon Memorial Secondary School</t>
-  </si>
-  <si>
-    <t>(647) 502-3605</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>905-956-2182</t>
-  </si>
-  <si>
-    <t>Drishti Thakkar</t>
-  </si>
-  <si>
-    <t>drishti.thakkar@gmail.com</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="151">
   <si>
     <t>Port Credit Secondary</t>
   </si>
@@ -499,6 +260,249 @@
   </si>
   <si>
     <t>(647) 280-2192</t>
+  </si>
+  <si>
+    <t>Guelph Humber</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zakira</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>karbaryz@gmail.com</t>
+  </si>
+  <si>
+    <t>dezaya.joseph@hotmail.com </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>hspathan13@gmail.com</t>
+  </si>
+  <si>
+    <t>David Leeder Middle School</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nasra Nadeem </t>
+  </si>
+  <si>
+    <t>nasra.nadeem@hotmail.com</t>
+  </si>
+  <si>
+    <t>Uswa Zahoor</t>
+  </si>
+  <si>
+    <t>uswa.zahoor@hotmail.ca</t>
+  </si>
+  <si>
+    <t>Glenforest Secondary School</t>
+  </si>
+  <si>
+    <t>Michael Jackman</t>
+  </si>
+  <si>
+    <t>michaelericjackman@gmail.com</t>
+  </si>
+  <si>
+    <t>Ayesha Faizi</t>
+  </si>
+  <si>
+    <t>Ali Turab Lotia</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>aliturablotia@gmail.com</t>
+  </si>
+  <si>
+    <t>Paul Konieczny</t>
+  </si>
+  <si>
+    <t>647-217-2793</t>
+  </si>
+  <si>
+    <t>pkonieczny@rogers.com</t>
+  </si>
+  <si>
+    <t>UTM</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ayesha.f13@gmail.com</t>
+  </si>
+  <si>
+    <t>Vivian Li</t>
+  </si>
+  <si>
+    <t>vivi881121@gmail.com</t>
+  </si>
+  <si>
+    <t>Diya</t>
+  </si>
+  <si>
+    <t>diyakamath@yahoo.ca</t>
+  </si>
+  <si>
+    <t>Stephen Lewis Secondary</t>
+  </si>
+  <si>
+    <t>David Suzuki Secondary</t>
+  </si>
+  <si>
+    <t>Contact Number</t>
+  </si>
+  <si>
+    <t>annie.195@hotmail.com</t>
+  </si>
+  <si>
+    <t>fatehhayer1999@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> hawkstar@live.ca</t>
+  </si>
+  <si>
+    <t>mikayla_december@outlook.com</t>
+  </si>
+  <si>
+    <t>imranshaista@hotmail.com</t>
+  </si>
+  <si>
+    <t>sundaram_balas@yahoo.ca</t>
+  </si>
+  <si>
+    <t>taimoorgul98@gmail.com</t>
+  </si>
+  <si>
+    <t>mmdj360@gmail.com</t>
+  </si>
+  <si>
+    <t>Xenwraith@gmail.com</t>
+  </si>
+  <si>
+    <t>416-737-7706 / 647-767-9601</t>
+  </si>
+  <si>
+    <t>416-738-3281</t>
+  </si>
+  <si>
+    <t>Drive</t>
+  </si>
+  <si>
+    <t>Syed Abdullah Hussain</t>
+  </si>
+  <si>
+    <t>abd_pisces@live.com</t>
+  </si>
+  <si>
+    <t>Anisha Akhtar</t>
+  </si>
+  <si>
+    <t>York University</t>
+  </si>
+  <si>
+    <t>Fateh Hayer</t>
+  </si>
+  <si>
+    <t>David Suzuki Secondary School, Brampton</t>
+  </si>
+  <si>
+    <t>(647) 822-7274</t>
+  </si>
+  <si>
+    <t>Ascension of Our Lord</t>
+  </si>
+  <si>
+    <t>905 405 9413</t>
+  </si>
+  <si>
+    <t>905 612 8353</t>
+  </si>
+  <si>
+    <t>647-997-0852</t>
+  </si>
+  <si>
+    <t>Vigil Vincent</t>
+  </si>
+  <si>
+    <t>vigiljoe24@gmail.com</t>
+  </si>
+  <si>
+    <t>(437) 580-0905 / (905) 205-0304</t>
+  </si>
+  <si>
+    <t>aritankovic@gmail.com</t>
+  </si>
+  <si>
+    <t>Armin Tankovic</t>
+  </si>
+  <si>
+    <t>Dezaya Joseph</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brandon Prakash</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pabdeep</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lincoln Alexander Secondary School. </t>
+  </si>
+  <si>
+    <t>brandon.prakash@hotmail.com</t>
+  </si>
+  <si>
+    <t> 905 678 6526</t>
+  </si>
+  <si>
+    <t>905 956 1163</t>
+  </si>
+  <si>
+    <t>Lincoln Alexander Secondary School. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>panesar.panesar@gmail.com</t>
+  </si>
+  <si>
+    <t>St. Joseph</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>jetaix01@yahoo.ca</t>
+  </si>
+  <si>
+    <t>fawaddv@gmail.com</t>
+  </si>
+  <si>
+    <t>Taimoor</t>
+  </si>
+  <si>
+    <t>647-300-0101 / 647 960 1002</t>
+  </si>
+  <si>
+    <t>tanvi1111@hotmail.com</t>
+  </si>
+  <si>
+    <t>Tanvi Mehta</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gordon Graydon Memorial Secondary School</t>
+  </si>
+  <si>
+    <t>(647) 502-3605</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>905-956-2182</t>
+  </si>
+  <si>
+    <t>Drishti Thakkar</t>
+  </si>
+  <si>
+    <t>drishti.thakkar@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -619,74 +623,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -703,7 +639,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="78DC78"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -981,53 +917,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>123</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>124</v>
+        <v>48</v>
       </c>
       <c r="C1" t="s">
-        <v>125</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>129</v>
+        <v>53</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>101</v>
       </c>
       <c r="F1" t="s">
-        <v>38</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>51</v>
       </c>
       <c r="C2">
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
+        <v>54</v>
       </c>
       <c r="E2" s="2">
         <v>6472445427</v>
@@ -1038,27 +974,27 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>55</v>
       </c>
       <c r="C3">
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>130</v>
+        <v>54</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>37</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>133</v>
+        <v>57</v>
       </c>
       <c r="C4">
         <v>17</v>
@@ -1069,50 +1005,50 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>135</v>
+        <v>59</v>
       </c>
       <c r="C5">
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>84</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>60</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>78</v>
       </c>
       <c r="C6">
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>4</v>
+        <v>79</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>36</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>81</v>
       </c>
       <c r="C7">
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="E7" s="2">
         <v>6478600426</v>
@@ -1120,16 +1056,16 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="C8">
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
       <c r="E8" s="2">
         <v>6477678445</v>
@@ -1137,33 +1073,33 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>86</v>
       </c>
       <c r="C9">
         <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>130</v>
+        <v>54</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>120</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>87</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>94</v>
       </c>
       <c r="C10">
         <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>130</v>
+        <v>54</v>
       </c>
       <c r="E10" s="2">
         <v>4166711521</v>
@@ -1171,16 +1107,16 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>96</v>
       </c>
       <c r="C11">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
       <c r="E11" s="2">
         <v>6478295824</v>
@@ -1188,10 +1124,10 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>97</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>98</v>
       </c>
       <c r="C12">
         <v>14</v>
@@ -1200,16 +1136,16 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>116</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="C13">
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>42</v>
+        <v>117</v>
       </c>
       <c r="E13" s="2">
         <v>9056731538</v>
@@ -1217,79 +1153,79 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>118</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>103</v>
       </c>
       <c r="C14">
         <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>44</v>
+        <v>119</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="B15" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
       <c r="C15">
         <v>15</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>48</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="B16" t="s">
-        <v>30</v>
+        <v>105</v>
       </c>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5">
       <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>106</v>
       </c>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5">
       <c r="B18" t="s">
-        <v>32</v>
+        <v>107</v>
       </c>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>142</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>108</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>73</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="B20" s="1" t="s">
-        <v>34</v>
+        <v>109</v>
       </c>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5">
       <c r="B21" t="s">
-        <v>35</v>
+        <v>110</v>
       </c>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>114</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>115</v>
       </c>
       <c r="C22">
         <v>14</v>
@@ -1298,16 +1234,16 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>65</v>
+        <v>140</v>
       </c>
       <c r="C23">
         <v>13</v>
       </c>
       <c r="D23" t="s">
-        <v>101</v>
+        <v>25</v>
       </c>
       <c r="E23">
         <v>9054619350</v>
@@ -1315,16 +1251,16 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>116</v>
+        <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>141</v>
       </c>
       <c r="C24">
         <v>13</v>
       </c>
       <c r="D24" t="s">
-        <v>117</v>
+        <v>41</v>
       </c>
       <c r="E24">
         <v>6474061810</v>
@@ -1332,58 +1268,58 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="5" t="s">
-        <v>74</v>
+        <v>149</v>
       </c>
       <c r="B25" t="s">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="C25">
         <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>77</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="5" t="s">
-        <v>78</v>
+        <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>79</v>
+        <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>130</v>
+        <v>54</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>80</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>102</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>103</v>
+        <v>27</v>
       </c>
       <c r="D27" t="s">
-        <v>130</v>
+        <v>54</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>104</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>113</v>
+        <v>37</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>107</v>
+        <v>31</v>
       </c>
       <c r="D28" t="s">
-        <v>108</v>
+        <v>32</v>
       </c>
       <c r="E28">
         <v>9054860232</v>
@@ -1391,7 +1327,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="B29" t="s">
-        <v>114</v>
+        <v>38</v>
       </c>
       <c r="E29">
         <v>9059131216</v>
@@ -1399,87 +1335,87 @@
     </row>
     <row r="30" spans="1:5">
       <c r="B30" t="s">
-        <v>115</v>
+        <v>39</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>118</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="B31" t="s">
-        <v>119</v>
+        <v>43</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>121</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="B32" t="s">
-        <v>122</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>109</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>110</v>
+        <v>34</v>
       </c>
       <c r="D33" t="s">
-        <v>111</v>
+        <v>35</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>112</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>82</v>
+        <v>6</v>
       </c>
       <c r="D34" t="s">
-        <v>130</v>
+        <v>54</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>83</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>85</v>
+        <v>9</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>87</v>
+        <v>11</v>
       </c>
       <c r="D35" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="E35">
         <v>4169535569</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="17.25">
+    <row r="36" spans="1:5" ht="16">
       <c r="A36" t="s">
-        <v>88</v>
+        <v>12</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>89</v>
+        <v>13</v>
       </c>
       <c r="C36">
         <v>21</v>
       </c>
       <c r="D36" t="s">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="E36" t="s">
-        <v>91</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="B37" s="7" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="E37">
         <v>4167233866</v>
@@ -1487,243 +1423,243 @@
     </row>
     <row r="38" spans="1:5">
       <c r="B38" s="7" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>94</v>
+        <v>18</v>
       </c>
       <c r="C39">
         <v>15</v>
       </c>
       <c r="D39" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="17.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="16">
       <c r="A40" t="s">
-        <v>95</v>
+        <v>19</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>96</v>
+        <v>20</v>
       </c>
       <c r="C40">
         <v>21</v>
       </c>
       <c r="D40" t="s">
-        <v>99</v>
+        <v>23</v>
       </c>
       <c r="E40" t="s">
-        <v>45</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>70</v>
+        <v>145</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>69</v>
+        <v>144</v>
       </c>
       <c r="C41">
         <v>14</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>71</v>
+        <v>146</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="18.75">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="19">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>88</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>14</v>
+        <v>89</v>
       </c>
       <c r="D42" t="s">
-        <v>18</v>
+        <v>93</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="16.5">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="16">
       <c r="A43" s="11" t="s">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="D43" t="s">
-        <v>18</v>
+        <v>93</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="18.75">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="19">
       <c r="A44" t="s">
-        <v>106</v>
+        <v>30</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>105</v>
+        <v>29</v>
       </c>
       <c r="C44">
         <v>13</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>46</v>
+        <v>121</v>
       </c>
       <c r="E44" t="s">
-        <v>47</v>
+        <v>122</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>50</v>
+        <v>125</v>
       </c>
       <c r="B45" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="C45">
         <v>17</v>
       </c>
       <c r="D45" t="s">
-        <v>46</v>
+        <v>121</v>
       </c>
       <c r="E45" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
+        <v>129</v>
+      </c>
+      <c r="B46" t="s">
+        <v>128</v>
+      </c>
+      <c r="D46" t="s">
         <v>54</v>
-      </c>
-      <c r="B46" t="s">
-        <v>53</v>
-      </c>
-      <c r="D46" t="s">
-        <v>130</v>
       </c>
       <c r="E46">
         <v>6478227275</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="18.75">
+    <row r="47" spans="1:5" ht="19">
       <c r="A47" t="s">
-        <v>55</v>
+        <v>130</v>
       </c>
       <c r="B47" t="s">
-        <v>2</v>
+        <v>77</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>58</v>
+        <v>133</v>
       </c>
       <c r="E47" s="10">
         <v>6476336597</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="18.75">
+    <row r="48" spans="1:5" ht="19">
       <c r="A48" t="s">
-        <v>56</v>
+        <v>131</v>
       </c>
       <c r="B48" t="s">
-        <v>59</v>
+        <v>134</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>58</v>
+        <v>133</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="18.75">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="19">
       <c r="A49" t="s">
-        <v>57</v>
+        <v>132</v>
       </c>
       <c r="B49" t="s">
-        <v>63</v>
+        <v>138</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>62</v>
+        <v>137</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="18.75">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="19">
       <c r="A50" t="s">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>1</v>
+        <v>76</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>64</v>
+        <v>139</v>
       </c>
       <c r="E50" s="10">
         <v>6473626012</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="18.75">
+    <row r="51" spans="1:5" ht="19">
       <c r="A51" t="s">
-        <v>137</v>
+        <v>61</v>
       </c>
       <c r="B51" t="s">
-        <v>138</v>
+        <v>62</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>139</v>
+        <v>63</v>
       </c>
       <c r="E51" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="18.75">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="19">
       <c r="A52" t="s">
-        <v>141</v>
+        <v>65</v>
       </c>
       <c r="B52" t="s">
-        <v>142</v>
+        <v>66</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>143</v>
+        <v>67</v>
       </c>
       <c r="E52" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="18.75">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="19">
       <c r="A53" t="s">
-        <v>145</v>
+        <v>69</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>148</v>
+        <v>72</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="E53">
         <v>6477195000</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="18.75">
+    <row r="54" spans="1:5" ht="19">
       <c r="A54" t="s">
-        <v>146</v>
+        <v>70</v>
       </c>
       <c r="B54" t="s">
-        <v>147</v>
+        <v>71</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>130</v>
+        <v>54</v>
       </c>
       <c r="E54" t="s">
-        <v>149</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1746,7 +1682,6 @@
     <hyperlink ref="B53" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1756,12 +1691,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1773,12 +1708,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Kayla missing info added
</commit_message>
<xml_diff>
--- a/campaign/VolunteerInformation.xlsx
+++ b/campaign/VolunteerInformation.xlsx
@@ -21,7 +21,250 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="154">
+  <si>
+    <t>(647) 721-8251</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>dezaya.joseph@hotmail.com </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>hspathan13@gmail.com</t>
+  </si>
+  <si>
+    <t>David Leeder Middle School</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nasra Nadeem </t>
+  </si>
+  <si>
+    <t>nasra.nadeem@hotmail.com</t>
+  </si>
+  <si>
+    <t>Uswa Zahoor</t>
+  </si>
+  <si>
+    <t>uswa.zahoor@hotmail.ca</t>
+  </si>
+  <si>
+    <t>Glenforest Secondary School</t>
+  </si>
+  <si>
+    <t>Michael Jackman</t>
+  </si>
+  <si>
+    <t>michaelericjackman@gmail.com</t>
+  </si>
+  <si>
+    <t>Ayesha Faizi</t>
+  </si>
+  <si>
+    <t>Ali Turab Lotia</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>aliturablotia@gmail.com</t>
+  </si>
+  <si>
+    <t>Paul Konieczny</t>
+  </si>
+  <si>
+    <t>647-217-2793</t>
+  </si>
+  <si>
+    <t>pkonieczny@rogers.com</t>
+  </si>
+  <si>
+    <t>UTM</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ayesha.f13@gmail.com</t>
+  </si>
+  <si>
+    <t>Vivian Li</t>
+  </si>
+  <si>
+    <t>vivi881121@gmail.com</t>
+  </si>
+  <si>
+    <t>Diya</t>
+  </si>
+  <si>
+    <t>diyakamath@yahoo.ca</t>
+  </si>
+  <si>
+    <t>Stephen Lewis Secondary</t>
+  </si>
+  <si>
+    <t>David Suzuki Secondary</t>
+  </si>
+  <si>
+    <t>Contact Number</t>
+  </si>
+  <si>
+    <t>annie.195@hotmail.com</t>
+  </si>
+  <si>
+    <t>fatehhayer1999@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> hawkstar@live.ca</t>
+  </si>
+  <si>
+    <t>mikayla_december@outlook.com</t>
+  </si>
+  <si>
+    <t>imranshaista@hotmail.com</t>
+  </si>
+  <si>
+    <t>sundaram_balas@yahoo.ca</t>
+  </si>
+  <si>
+    <t>taimoorgul98@gmail.com</t>
+  </si>
+  <si>
+    <t>mmdj360@gmail.com</t>
+  </si>
+  <si>
+    <t>Xenwraith@gmail.com</t>
+  </si>
+  <si>
+    <t>416-737-7706 / 647-767-9601</t>
+  </si>
+  <si>
+    <t>416-738-3281</t>
+  </si>
+  <si>
+    <t>Drive</t>
+  </si>
+  <si>
+    <t>Syed Abdullah Hussain</t>
+  </si>
+  <si>
+    <t>abd_pisces@live.com</t>
+  </si>
+  <si>
+    <t>Anisha Akhtar</t>
+  </si>
+  <si>
+    <t>York University</t>
+  </si>
+  <si>
+    <t>Fateh Hayer</t>
+  </si>
+  <si>
+    <t>David Suzuki Secondary School, Brampton</t>
+  </si>
+  <si>
+    <t>(647) 822-7274</t>
+  </si>
+  <si>
+    <t>Ascension of Our Lord</t>
+  </si>
+  <si>
+    <t>905 405 9413</t>
+  </si>
+  <si>
+    <t>905 612 8353</t>
+  </si>
+  <si>
+    <t>647-997-0852</t>
+  </si>
+  <si>
+    <t>Vigil Vincent</t>
+  </si>
+  <si>
+    <t>vigiljoe24@gmail.com</t>
+  </si>
+  <si>
+    <t>(437) 580-0905 / (905) 205-0304</t>
+  </si>
+  <si>
+    <t>aritankovic@gmail.com</t>
+  </si>
+  <si>
+    <t>Armin Tankovic</t>
+  </si>
+  <si>
+    <t>Dezaya Joseph</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brandon Prakash</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pabdeep</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lincoln Alexander Secondary School. </t>
+  </si>
+  <si>
+    <t>brandon.prakash@hotmail.com</t>
+  </si>
+  <si>
+    <t> 905 678 6526</t>
+  </si>
+  <si>
+    <t>905 956 1163</t>
+  </si>
+  <si>
+    <t>Lincoln Alexander Secondary School. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>panesar.panesar@gmail.com</t>
+  </si>
+  <si>
+    <t>St. Joseph</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>jetaix01@yahoo.ca</t>
+  </si>
+  <si>
+    <t>fawaddv@gmail.com</t>
+  </si>
+  <si>
+    <t>Taimoor</t>
+  </si>
+  <si>
+    <t>647-300-0101 / 647 960 1002</t>
+  </si>
+  <si>
+    <t>tanvi1111@hotmail.com</t>
+  </si>
+  <si>
+    <t>Tanvi Mehta</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gordon Graydon Memorial Secondary School</t>
+  </si>
+  <si>
+    <t>(647) 502-3605</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>905-956-2182</t>
+  </si>
+  <si>
+    <t>Drishti Thakkar</t>
+  </si>
+  <si>
+    <t>drishti.thakkar@gmail.com</t>
+  </si>
+  <si>
+    <t>Kayla</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>k.beckford@live.ca</t>
+  </si>
   <si>
     <t>Port Credit Secondary</t>
   </si>
@@ -271,238 +514,6 @@
   </si>
   <si>
     <t>karbaryz@gmail.com</t>
-  </si>
-  <si>
-    <t>dezaya.joseph@hotmail.com </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>hspathan13@gmail.com</t>
-  </si>
-  <si>
-    <t>David Leeder Middle School</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nasra Nadeem </t>
-  </si>
-  <si>
-    <t>nasra.nadeem@hotmail.com</t>
-  </si>
-  <si>
-    <t>Uswa Zahoor</t>
-  </si>
-  <si>
-    <t>uswa.zahoor@hotmail.ca</t>
-  </si>
-  <si>
-    <t>Glenforest Secondary School</t>
-  </si>
-  <si>
-    <t>Michael Jackman</t>
-  </si>
-  <si>
-    <t>michaelericjackman@gmail.com</t>
-  </si>
-  <si>
-    <t>Ayesha Faizi</t>
-  </si>
-  <si>
-    <t>Ali Turab Lotia</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>aliturablotia@gmail.com</t>
-  </si>
-  <si>
-    <t>Paul Konieczny</t>
-  </si>
-  <si>
-    <t>647-217-2793</t>
-  </si>
-  <si>
-    <t>pkonieczny@rogers.com</t>
-  </si>
-  <si>
-    <t>UTM</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ayesha.f13@gmail.com</t>
-  </si>
-  <si>
-    <t>Vivian Li</t>
-  </si>
-  <si>
-    <t>vivi881121@gmail.com</t>
-  </si>
-  <si>
-    <t>Diya</t>
-  </si>
-  <si>
-    <t>diyakamath@yahoo.ca</t>
-  </si>
-  <si>
-    <t>Stephen Lewis Secondary</t>
-  </si>
-  <si>
-    <t>David Suzuki Secondary</t>
-  </si>
-  <si>
-    <t>Contact Number</t>
-  </si>
-  <si>
-    <t>annie.195@hotmail.com</t>
-  </si>
-  <si>
-    <t>fatehhayer1999@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> hawkstar@live.ca</t>
-  </si>
-  <si>
-    <t>mikayla_december@outlook.com</t>
-  </si>
-  <si>
-    <t>imranshaista@hotmail.com</t>
-  </si>
-  <si>
-    <t>sundaram_balas@yahoo.ca</t>
-  </si>
-  <si>
-    <t>taimoorgul98@gmail.com</t>
-  </si>
-  <si>
-    <t>mmdj360@gmail.com</t>
-  </si>
-  <si>
-    <t>Xenwraith@gmail.com</t>
-  </si>
-  <si>
-    <t>416-737-7706 / 647-767-9601</t>
-  </si>
-  <si>
-    <t>416-738-3281</t>
-  </si>
-  <si>
-    <t>Drive</t>
-  </si>
-  <si>
-    <t>Syed Abdullah Hussain</t>
-  </si>
-  <si>
-    <t>abd_pisces@live.com</t>
-  </si>
-  <si>
-    <t>Anisha Akhtar</t>
-  </si>
-  <si>
-    <t>York University</t>
-  </si>
-  <si>
-    <t>Fateh Hayer</t>
-  </si>
-  <si>
-    <t>David Suzuki Secondary School, Brampton</t>
-  </si>
-  <si>
-    <t>(647) 822-7274</t>
-  </si>
-  <si>
-    <t>Ascension of Our Lord</t>
-  </si>
-  <si>
-    <t>905 405 9413</t>
-  </si>
-  <si>
-    <t>905 612 8353</t>
-  </si>
-  <si>
-    <t>647-997-0852</t>
-  </si>
-  <si>
-    <t>Vigil Vincent</t>
-  </si>
-  <si>
-    <t>vigiljoe24@gmail.com</t>
-  </si>
-  <si>
-    <t>(437) 580-0905 / (905) 205-0304</t>
-  </si>
-  <si>
-    <t>aritankovic@gmail.com</t>
-  </si>
-  <si>
-    <t>Armin Tankovic</t>
-  </si>
-  <si>
-    <t>Dezaya Joseph</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Brandon Prakash</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pabdeep</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lincoln Alexander Secondary School. </t>
-  </si>
-  <si>
-    <t>brandon.prakash@hotmail.com</t>
-  </si>
-  <si>
-    <t> 905 678 6526</t>
-  </si>
-  <si>
-    <t>905 956 1163</t>
-  </si>
-  <si>
-    <t>Lincoln Alexander Secondary School. </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>panesar.panesar@gmail.com</t>
-  </si>
-  <si>
-    <t>St. Joseph</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>jetaix01@yahoo.ca</t>
-  </si>
-  <si>
-    <t>fawaddv@gmail.com</t>
-  </si>
-  <si>
-    <t>Taimoor</t>
-  </si>
-  <si>
-    <t>647-300-0101 / 647 960 1002</t>
-  </si>
-  <si>
-    <t>tanvi1111@hotmail.com</t>
-  </si>
-  <si>
-    <t>Tanvi Mehta</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gordon Graydon Memorial Secondary School</t>
-  </si>
-  <si>
-    <t>(647) 502-3605</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>905-956-2182</t>
-  </si>
-  <si>
-    <t>Drishti Thakkar</t>
-  </si>
-  <si>
-    <t>drishti.thakkar@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -918,10 +929,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -934,36 +945,36 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>124</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>125</v>
       </c>
       <c r="C1" t="s">
-        <v>49</v>
+        <v>126</v>
       </c>
       <c r="D1" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="E1" t="s">
-        <v>101</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>113</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>128</v>
       </c>
       <c r="C2">
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>131</v>
       </c>
       <c r="E2" s="2">
         <v>6472445427</v>
@@ -974,27 +985,27 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>129</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>132</v>
       </c>
       <c r="C3">
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>131</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>112</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>133</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>134</v>
       </c>
       <c r="C4">
         <v>17</v>
@@ -1005,50 +1016,50 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>135</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>136</v>
       </c>
       <c r="C5">
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>99</v>
+        <v>23</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>8</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>137</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>78</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>79</v>
+        <v>3</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>111</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="E7" s="2">
         <v>6478600426</v>
@@ -1056,16 +1067,16 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>84</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2">
         <v>6477678445</v>
@@ -1073,33 +1084,33 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>85</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>131</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>44</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>87</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>94</v>
+        <v>18</v>
       </c>
       <c r="C10">
         <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>54</v>
+        <v>131</v>
       </c>
       <c r="E10" s="2">
         <v>4166711521</v>
@@ -1107,16 +1118,16 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>96</v>
+        <v>20</v>
       </c>
       <c r="C11">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>84</v>
+        <v>8</v>
       </c>
       <c r="E11" s="2">
         <v>6478295824</v>
@@ -1124,10 +1135,10 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>98</v>
+        <v>22</v>
       </c>
       <c r="C12">
         <v>14</v>
@@ -1136,16 +1147,16 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>116</v>
+        <v>40</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>102</v>
+        <v>26</v>
       </c>
       <c r="C13">
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>117</v>
+        <v>41</v>
       </c>
       <c r="E13" s="2">
         <v>9056731538</v>
@@ -1153,79 +1164,79 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>118</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>103</v>
+        <v>27</v>
       </c>
       <c r="C14">
         <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>119</v>
+        <v>43</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>143</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="B15" t="s">
-        <v>104</v>
+        <v>28</v>
       </c>
       <c r="C15">
         <v>15</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>123</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="B16" t="s">
-        <v>105</v>
+        <v>29</v>
       </c>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5">
       <c r="B17" s="1" t="s">
-        <v>106</v>
+        <v>30</v>
       </c>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5">
       <c r="B18" t="s">
-        <v>107</v>
+        <v>31</v>
       </c>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>142</v>
+        <v>66</v>
       </c>
       <c r="B19" t="s">
-        <v>108</v>
+        <v>32</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>148</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="B20" s="1" t="s">
-        <v>109</v>
+        <v>33</v>
       </c>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5">
       <c r="B21" t="s">
-        <v>110</v>
+        <v>34</v>
       </c>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>114</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>115</v>
+        <v>39</v>
       </c>
       <c r="C22">
         <v>14</v>
@@ -1234,16 +1245,16 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>101</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>140</v>
+        <v>64</v>
       </c>
       <c r="C23">
         <v>13</v>
       </c>
       <c r="D23" t="s">
-        <v>25</v>
+        <v>102</v>
       </c>
       <c r="E23">
         <v>9054619350</v>
@@ -1251,16 +1262,16 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>117</v>
       </c>
       <c r="B24" t="s">
-        <v>141</v>
+        <v>65</v>
       </c>
       <c r="C24">
         <v>13</v>
       </c>
       <c r="D24" t="s">
-        <v>41</v>
+        <v>118</v>
       </c>
       <c r="E24">
         <v>6474061810</v>
@@ -1268,58 +1279,58 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="5" t="s">
-        <v>149</v>
+        <v>73</v>
       </c>
       <c r="B25" t="s">
-        <v>150</v>
+        <v>74</v>
       </c>
       <c r="C25">
         <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>1</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="5" t="s">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
-        <v>3</v>
+        <v>80</v>
       </c>
       <c r="D26" t="s">
-        <v>54</v>
+        <v>131</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>4</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>103</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
+        <v>104</v>
       </c>
       <c r="D27" t="s">
-        <v>54</v>
+        <v>131</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>28</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>114</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>31</v>
+        <v>108</v>
       </c>
       <c r="D28" t="s">
-        <v>32</v>
+        <v>109</v>
       </c>
       <c r="E28">
         <v>9054860232</v>
@@ -1327,7 +1338,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="B29" t="s">
-        <v>38</v>
+        <v>115</v>
       </c>
       <c r="E29">
         <v>9059131216</v>
@@ -1335,62 +1346,62 @@
     </row>
     <row r="30" spans="1:5">
       <c r="B30" t="s">
-        <v>39</v>
+        <v>116</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>42</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="B31" t="s">
-        <v>43</v>
+        <v>120</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="B32" t="s">
-        <v>46</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>110</v>
       </c>
       <c r="B33" t="s">
-        <v>34</v>
+        <v>111</v>
       </c>
       <c r="D33" t="s">
-        <v>35</v>
+        <v>112</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>36</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>5</v>
+        <v>82</v>
       </c>
       <c r="B34" t="s">
-        <v>6</v>
+        <v>83</v>
       </c>
       <c r="D34" t="s">
-        <v>54</v>
+        <v>131</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>9</v>
+        <v>86</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>11</v>
+        <v>88</v>
       </c>
       <c r="D35" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="E35">
         <v>4169535569</v>
@@ -1398,24 +1409,24 @@
     </row>
     <row r="36" spans="1:5" ht="16">
       <c r="A36" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>13</v>
+        <v>90</v>
       </c>
       <c r="C36">
         <v>21</v>
       </c>
       <c r="D36" t="s">
-        <v>14</v>
+        <v>91</v>
       </c>
       <c r="E36" t="s">
-        <v>15</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="B37" s="7" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="E37">
         <v>4167233866</v>
@@ -1423,128 +1434,128 @@
     </row>
     <row r="38" spans="1:5">
       <c r="B38" s="7" t="s">
-        <v>17</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>21</v>
+        <v>98</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>18</v>
+        <v>95</v>
       </c>
       <c r="C39">
         <v>15</v>
       </c>
       <c r="D39" t="s">
-        <v>22</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="16">
       <c r="A40" t="s">
-        <v>19</v>
+        <v>96</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>20</v>
+        <v>97</v>
       </c>
       <c r="C40">
         <v>21</v>
       </c>
       <c r="D40" t="s">
-        <v>23</v>
+        <v>100</v>
       </c>
       <c r="E40" t="s">
-        <v>120</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>145</v>
+        <v>69</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>144</v>
+        <v>68</v>
       </c>
       <c r="C41">
         <v>14</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>146</v>
+        <v>70</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>147</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="19">
       <c r="A42" t="s">
-        <v>88</v>
+        <v>12</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>89</v>
+        <v>13</v>
       </c>
       <c r="D42" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>124</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="16">
       <c r="A43" s="11" t="s">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="D43" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>91</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="19">
       <c r="A44" t="s">
-        <v>30</v>
+        <v>107</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>29</v>
+        <v>106</v>
       </c>
       <c r="C44">
         <v>13</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>121</v>
+        <v>45</v>
       </c>
       <c r="E44" t="s">
-        <v>122</v>
+        <v>46</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>125</v>
+        <v>49</v>
       </c>
       <c r="B45" t="s">
-        <v>126</v>
+        <v>50</v>
       </c>
       <c r="C45">
         <v>17</v>
       </c>
       <c r="D45" t="s">
-        <v>121</v>
+        <v>45</v>
       </c>
       <c r="E45" t="s">
-        <v>127</v>
+        <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>129</v>
+        <v>53</v>
       </c>
       <c r="B46" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="D46" t="s">
-        <v>54</v>
+        <v>131</v>
       </c>
       <c r="E46">
         <v>6478227275</v>
@@ -1552,13 +1563,13 @@
     </row>
     <row r="47" spans="1:5" ht="19">
       <c r="A47" t="s">
-        <v>130</v>
+        <v>54</v>
       </c>
       <c r="B47" t="s">
-        <v>77</v>
+        <v>1</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>133</v>
+        <v>57</v>
       </c>
       <c r="E47" s="10">
         <v>6476336597</v>
@@ -1566,41 +1577,41 @@
     </row>
     <row r="48" spans="1:5" ht="19">
       <c r="A48" t="s">
-        <v>131</v>
+        <v>55</v>
       </c>
       <c r="B48" t="s">
-        <v>134</v>
+        <v>58</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>133</v>
+        <v>57</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>135</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="19">
       <c r="A49" t="s">
-        <v>132</v>
+        <v>56</v>
       </c>
       <c r="B49" t="s">
-        <v>138</v>
+        <v>62</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>137</v>
+        <v>61</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>136</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="19">
       <c r="A50" t="s">
-        <v>75</v>
+        <v>152</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>76</v>
+        <v>153</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>139</v>
+        <v>63</v>
       </c>
       <c r="E50" s="10">
         <v>6473626012</v>
@@ -1608,41 +1619,41 @@
     </row>
     <row r="51" spans="1:5" ht="19">
       <c r="A51" t="s">
-        <v>61</v>
+        <v>138</v>
       </c>
       <c r="B51" t="s">
-        <v>62</v>
+        <v>139</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>63</v>
+        <v>140</v>
       </c>
       <c r="E51" t="s">
-        <v>64</v>
+        <v>141</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="19">
       <c r="A52" t="s">
-        <v>65</v>
+        <v>142</v>
       </c>
       <c r="B52" t="s">
-        <v>66</v>
+        <v>143</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>67</v>
+        <v>144</v>
       </c>
       <c r="E52" t="s">
-        <v>68</v>
+        <v>145</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="19">
       <c r="A53" t="s">
-        <v>69</v>
+        <v>146</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>72</v>
+        <v>149</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>74</v>
+        <v>151</v>
       </c>
       <c r="E53">
         <v>6477195000</v>
@@ -1650,16 +1661,27 @@
     </row>
     <row r="54" spans="1:5" ht="19">
       <c r="A54" t="s">
-        <v>70</v>
+        <v>147</v>
       </c>
       <c r="B54" t="s">
-        <v>71</v>
+        <v>148</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>54</v>
+        <v>131</v>
       </c>
       <c r="E54" t="s">
-        <v>73</v>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>75</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E55" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1680,6 +1702,7 @@
     <hyperlink ref="B43" r:id="rId13"/>
     <hyperlink ref="B50" r:id="rId14"/>
     <hyperlink ref="B53" r:id="rId15"/>
+    <hyperlink ref="B55" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
update one new volunteer
update one new volunteer
</commit_message>
<xml_diff>
--- a/campaign/VolunteerInformation.xlsx
+++ b/campaign/VolunteerInformation.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="166">
   <si>
     <t>Zakira</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -543,6 +543,9 @@
   </si>
   <si>
     <t xml:space="preserve">dene1998@hotmail.com </t>
+  </si>
+  <si>
+    <t>saitejavankadari2009@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1026,10 +1029,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1838,6 +1841,14 @@
       </c>
       <c r="E59">
         <v>6472303827</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="18.75">
+      <c r="B60" t="s">
+        <v>165</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating additional volunteers information
updating additional volunteers information
</commit_message>
<xml_diff>
--- a/campaign/VolunteerInformation.xlsx
+++ b/campaign/VolunteerInformation.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="171">
   <si>
     <t>Zakira</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -549,6 +549,18 @@
   </si>
   <si>
     <t>BROKE HIS LEG</t>
+  </si>
+  <si>
+    <t>Sai</t>
+  </si>
+  <si>
+    <t>Janarth Kulenthiran</t>
+  </si>
+  <si>
+    <t>kulenthirankk@hotmail.com</t>
+  </si>
+  <si>
+    <t>905-813-9777 / 4167329912</t>
   </si>
 </sst>
 </file>
@@ -1032,10 +1044,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1851,11 +1863,31 @@
       </c>
     </row>
     <row r="60" spans="1:5" ht="18.75">
+      <c r="A60" t="s">
+        <v>167</v>
+      </c>
       <c r="B60" t="s">
         <v>165</v>
       </c>
       <c r="D60" s="10" t="s">
         <v>46</v>
+      </c>
+      <c r="E60">
+        <v>6477798466</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="18.75">
+      <c r="A61" t="s">
+        <v>168</v>
+      </c>
+      <c r="B61" t="s">
+        <v>169</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E61" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>